<commit_message>
Updated viz for Day 1.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 1: TITLE</t>
-  </si>
-  <si>
     <t>Day 2: TITLE</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>Day 25: TITLE</t>
+  </si>
+  <si>
+    <t>Day 1: The Tyranny of the Rocket Equation</t>
   </si>
 </sst>
 </file>
@@ -778,7 +778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -857,26 +859,34 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.6435185185185183E-3</v>
+      </c>
       <c r="D5" s="15">
         <f t="shared" ref="D5:D29" si="0">E5-C5</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="21"/>
+        <v>1.921296296296297E-3</v>
+      </c>
+      <c r="E5" s="16">
+        <v>3.5648148148148154E-3</v>
+      </c>
+      <c r="F5" s="21">
+        <v>2.7546296296296294E-3</v>
+      </c>
       <c r="G5" s="21">
         <f t="shared" ref="G5:G29" si="1">E5-F5</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="28"/>
+        <v>8.1018518518518592E-4</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>7</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="15">
@@ -895,7 +905,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="15">
@@ -914,7 +924,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="15">
@@ -933,7 +943,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="15">
@@ -952,7 +962,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15">
@@ -971,7 +981,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -990,7 +1000,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1009,7 +1019,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1028,7 +1038,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1047,7 +1057,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1066,7 +1076,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1085,7 +1095,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1104,7 +1114,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1123,7 +1133,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1142,7 +1152,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1161,7 +1171,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1180,7 +1190,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1199,7 +1209,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1218,7 +1228,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1237,7 +1247,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1256,7 +1266,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1275,7 +1285,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1294,7 +1304,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1313,7 +1323,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">
@@ -1355,9 +1365,9 @@
       <c r="D32" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="23" t="e">
+      <c r="E32" s="23">
         <f>MEDIAN(E5:E29)</f>
-        <v>#NUM!</v>
+        <v>3.5648148148148154E-3</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
@@ -1366,9 +1376,9 @@
       <c r="D33" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="23" t="e">
+      <c r="E33" s="23">
         <f>MEDIAN(E5,E6,E7,E8,E9,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29)</f>
-        <v>#NUM!</v>
+        <v>3.5648148148148154E-3</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>

</xml_diff>

<commit_message>
Updated viz for Day 2.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 2: TITLE</t>
-  </si>
-  <si>
     <t>Day 3: TITLE</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>Day 1: The Tyranny of the Rocket Equation</t>
+  </si>
+  <si>
+    <t>Day 2: 1202 Program Alarm</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -886,26 +886,34 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C6" s="2">
+        <v>6.782407407407408E-3</v>
+      </c>
       <c r="D6" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="21"/>
+        <v>5.8449074074074072E-3</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1.2627314814814815E-2</v>
+      </c>
+      <c r="F6" s="21">
+        <v>9.4444444444444445E-3</v>
+      </c>
       <c r="G6" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="28"/>
+        <v>3.1828703703703706E-3</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>9</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="15">
@@ -924,7 +932,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="15">
@@ -943,7 +951,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="15">
@@ -962,7 +970,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15">
@@ -981,7 +989,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1000,7 +1008,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1019,7 +1027,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1038,7 +1046,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1057,7 +1065,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1076,7 +1084,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1095,7 +1103,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1114,7 +1122,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1133,7 +1141,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1152,7 +1160,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1171,7 +1179,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1190,7 +1198,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1209,7 +1217,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1228,7 +1236,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1247,7 +1255,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1266,7 +1274,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1285,7 +1293,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1304,7 +1312,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1323,7 +1331,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">
@@ -1367,7 +1375,7 @@
       </c>
       <c r="E32" s="23">
         <f>MEDIAN(E5:E29)</f>
-        <v>3.5648148148148154E-3</v>
+        <v>8.0960648148148146E-3</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
@@ -1378,7 +1386,7 @@
       </c>
       <c r="E33" s="23">
         <f>MEDIAN(E5,E6,E7,E8,E9,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29)</f>
-        <v>3.5648148148148154E-3</v>
+        <v>8.0960648148148146E-3</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>

</xml_diff>

<commit_message>
Updated viz for Day 3.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 3: TITLE</t>
-  </si>
-  <si>
     <t>Day 4: TITLE</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>Day 2: 1202 Program Alarm</t>
+  </si>
+  <si>
+    <t>Day 3: Crossed Wires</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -886,7 +886,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -913,26 +913,34 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.5381944444444443E-2</v>
+      </c>
       <c r="D7" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="22"/>
+        <v>4.9189814814814842E-3</v>
+      </c>
+      <c r="E7" s="16">
+        <v>2.0300925925925927E-2</v>
+      </c>
+      <c r="F7" s="22">
+        <v>1.0902777777777777E-2</v>
+      </c>
       <c r="G7" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="16"/>
+        <v>9.3981481481481503E-3</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="15">
@@ -951,7 +959,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="15">
@@ -970,7 +978,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15">
@@ -989,7 +997,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1008,7 +1016,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1027,7 +1035,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1046,7 +1054,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1065,7 +1073,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1084,7 +1092,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1103,7 +1111,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1122,7 +1130,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1141,7 +1149,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1160,7 +1168,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1179,7 +1187,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1198,7 +1206,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1217,7 +1225,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1236,7 +1244,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1255,7 +1263,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1274,7 +1282,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1293,7 +1301,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1312,7 +1320,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1331,7 +1339,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">
@@ -1375,7 +1383,7 @@
       </c>
       <c r="E32" s="23">
         <f>MEDIAN(E5:E29)</f>
-        <v>8.0960648148148146E-3</v>
+        <v>1.2627314814814815E-2</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
@@ -1386,7 +1394,7 @@
       </c>
       <c r="E33" s="23">
         <f>MEDIAN(E5,E6,E7,E8,E9,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29)</f>
-        <v>8.0960648148148146E-3</v>
+        <v>1.2627314814814815E-2</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>

</xml_diff>

<commit_message>
Updated viz for Day 4.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 4: TITLE</t>
-  </si>
-  <si>
     <t>Day 5: TITLE</t>
   </si>
   <si>
@@ -231,6 +228,12 @@
   </si>
   <si>
     <t>Day 3: Crossed Wires</t>
+  </si>
+  <si>
+    <t>Day 4: Secure Container</t>
+  </si>
+  <si>
+    <t>11th</t>
   </si>
 </sst>
 </file>
@@ -779,7 +782,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +862,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -886,7 +889,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -913,7 +916,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -940,26 +943,34 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.37962962962963E-3</v>
+      </c>
       <c r="D8" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="22"/>
+        <v>1.9074074074074077E-2</v>
+      </c>
+      <c r="E8" s="16">
+        <v>2.2453703703703708E-2</v>
+      </c>
+      <c r="F8" s="22">
+        <v>5.0462962962962961E-3</v>
+      </c>
       <c r="G8" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="16"/>
+        <v>1.7407407407407413E-2</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="15">
@@ -978,7 +989,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15">
@@ -997,7 +1008,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1016,7 +1027,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1035,7 +1046,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1054,7 +1065,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1073,7 +1084,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1092,7 +1103,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1111,7 +1122,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1130,7 +1141,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1149,7 +1160,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1168,7 +1179,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1187,7 +1198,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1206,7 +1217,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1225,7 +1236,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1244,7 +1255,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1263,7 +1274,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1282,7 +1293,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1301,7 +1312,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1320,7 +1331,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1339,7 +1350,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">
@@ -1383,7 +1394,7 @@
       </c>
       <c r="E32" s="23">
         <f>MEDIAN(E5:E29)</f>
-        <v>1.2627314814814815E-2</v>
+        <v>1.6464120370370372E-2</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
@@ -1394,7 +1405,7 @@
       </c>
       <c r="E33" s="23">
         <f>MEDIAN(E5,E6,E7,E8,E9,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29)</f>
-        <v>1.2627314814814815E-2</v>
+        <v>1.6464120370370372E-2</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>

</xml_diff>

<commit_message>
Updated viz for Day 5.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 5: TITLE</t>
-  </si>
-  <si>
     <t>Day 6: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>11th</t>
+  </si>
+  <si>
+    <t>Day 5: Sunny with a Chance of Asteroids</t>
   </si>
 </sst>
 </file>
@@ -782,7 +782,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -889,7 +889,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -916,7 +916,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -943,7 +943,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -963,33 +963,41 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.9201388888888889E-2</v>
+      </c>
       <c r="D9" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="22"/>
+        <v>9.826388888888888E-3</v>
+      </c>
+      <c r="E9" s="16">
+        <v>2.9027777777777777E-2</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1.2395833333333335E-2</v>
+      </c>
       <c r="G9" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>1.6631944444444442E-2</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15">
@@ -1008,7 +1016,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1027,7 +1035,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1046,7 +1054,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1065,7 +1073,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1084,7 +1092,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1103,7 +1111,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1122,7 +1130,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1141,7 +1149,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1160,7 +1168,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1179,7 +1187,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1198,7 +1206,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1217,7 +1225,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1236,7 +1244,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1255,7 +1263,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1274,7 +1282,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1293,7 +1301,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1312,7 +1320,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1331,7 +1339,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1350,7 +1358,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">
@@ -1394,7 +1402,7 @@
       </c>
       <c r="E32" s="23">
         <f>MEDIAN(E5:E29)</f>
-        <v>1.6464120370370372E-2</v>
+        <v>2.0300925925925927E-2</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
@@ -1405,7 +1413,7 @@
       </c>
       <c r="E33" s="23">
         <f>MEDIAN(E5,E6,E7,E8,E9,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29)</f>
-        <v>1.6464120370370372E-2</v>
+        <v>2.0300925925925927E-2</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>

</xml_diff>

<commit_message>
Updated viz for Day 6.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 6: TITLE</t>
-  </si>
-  <si>
     <t>Day 7: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 5: Sunny with a Chance of Asteroids</t>
+  </si>
+  <si>
+    <t>Day 6: Universal Orbit Map</t>
   </si>
 </sst>
 </file>
@@ -782,7 +782,7 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -889,7 +889,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -916,7 +916,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -943,7 +943,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -963,14 +963,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -997,26 +997,34 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C10" s="2">
+        <v>6.7245370370370367E-3</v>
+      </c>
       <c r="D10" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="22"/>
+        <v>7.1180555555555572E-3</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1.3842592592592594E-2</v>
+      </c>
+      <c r="F10" s="22">
+        <v>1.3842592592592594E-2</v>
+      </c>
       <c r="G10" s="22">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10" s="16"/>
+      <c r="H10" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1035,7 +1043,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1054,7 +1062,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1073,7 +1081,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1092,7 +1100,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1111,7 +1119,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1130,7 +1138,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1149,7 +1157,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1168,7 +1176,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1187,7 +1195,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1206,7 +1214,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1225,7 +1233,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1244,7 +1252,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1263,7 +1271,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1282,7 +1290,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1301,7 +1309,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1320,7 +1328,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1339,7 +1347,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1358,7 +1366,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">
@@ -1402,19 +1410,14 @@
       </c>
       <c r="E32" s="23">
         <f>MEDIAN(E5:E29)</f>
-        <v>2.0300925925925927E-2</v>
+        <v>1.7071759259259259E-2</v>
       </c>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="23">
-        <f>MEDIAN(E5,E6,E7,E8,E9,E11,E12,E13,E14,E15,E16,E17,E18,E19,E20,E21,E22,E23,E24,E25,E26,E27,E28,E29)</f>
-        <v>2.0300925925925927E-2</v>
-      </c>
+      <c r="D33" s="24"/>
+      <c r="E33" s="23"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
     </row>

</xml_diff>

<commit_message>
Updated viz to also output individual sorted times of top scorers, for median comparisons.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
   <si>
     <t>Puzzle</t>
   </si>
@@ -234,6 +234,75 @@
   </si>
   <si>
     <t>Day 6: Universal Orbit Map</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Andrew Chang</t>
+  </si>
+  <si>
+    <t>Sam Holton</t>
+  </si>
+  <si>
+    <t>Elise Thorsen</t>
+  </si>
+  <si>
+    <t>Michael Herms</t>
+  </si>
+  <si>
+    <t>Taybin Rutkin</t>
+  </si>
+  <si>
+    <t>Shauna Revay</t>
+  </si>
+  <si>
+    <t>Eric Hughes</t>
+  </si>
+  <si>
+    <t>Matt Boehm</t>
+  </si>
+  <si>
+    <t>Lara Dedic</t>
+  </si>
+  <si>
+    <t>Rebecca Matous</t>
+  </si>
+  <si>
+    <t>Greg Fuller</t>
+  </si>
+  <si>
+    <t>Bradley Welsh</t>
+  </si>
+  <si>
+    <t>Jesse Florig</t>
+  </si>
+  <si>
+    <t>Robert Roger</t>
+  </si>
+  <si>
+    <t>Christopher Tibbetts</t>
+  </si>
+  <si>
+    <t>Nathan Shirley</t>
+  </si>
+  <si>
+    <t>Quintin DeGroot</t>
+  </si>
+  <si>
+    <t>Richard Bradley</t>
+  </si>
+  <si>
+    <t>Jonathan Skeate</t>
+  </si>
+  <si>
+    <t>Alan Carvajal</t>
+  </si>
+  <si>
+    <t>Brian Uri</t>
+  </si>
+  <si>
+    <t>Jeremy Glesner</t>
   </si>
 </sst>
 </file>
@@ -309,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -410,11 +479,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -478,6 +584,27 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:AK52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,9 +918,12 @@
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
     <col min="3" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="46" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -803,8 +933,36 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
+      <c r="AJ1" s="4"/>
+      <c r="AK1" s="4"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="8"/>
       <c r="C2" s="13"/>
@@ -818,8 +976,36 @@
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4"/>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="18"/>
       <c r="C3" s="10"/>
@@ -833,8 +1019,36 @@
         <v>17</v>
       </c>
       <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="4"/>
+      <c r="AE3" s="4"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="4"/>
+      <c r="AH3" s="4"/>
+      <c r="AI3" s="4"/>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -858,8 +1072,90 @@
         <v>46</v>
       </c>
       <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="36">
+        <v>1</v>
+      </c>
+      <c r="M4" s="36">
+        <v>2</v>
+      </c>
+      <c r="N4" s="36">
+        <v>3</v>
+      </c>
+      <c r="O4" s="36">
+        <v>4</v>
+      </c>
+      <c r="P4" s="36">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="36">
+        <v>6</v>
+      </c>
+      <c r="R4" s="36">
+        <v>7</v>
+      </c>
+      <c r="S4" s="36">
+        <v>8</v>
+      </c>
+      <c r="T4" s="36">
+        <v>9</v>
+      </c>
+      <c r="U4" s="36">
+        <v>10</v>
+      </c>
+      <c r="V4" s="36">
+        <v>11</v>
+      </c>
+      <c r="W4" s="36">
+        <v>12</v>
+      </c>
+      <c r="X4" s="36">
+        <v>13</v>
+      </c>
+      <c r="Y4" s="36">
+        <v>14</v>
+      </c>
+      <c r="Z4" s="36">
+        <v>15</v>
+      </c>
+      <c r="AA4" s="36">
+        <v>16</v>
+      </c>
+      <c r="AB4" s="36">
+        <v>17</v>
+      </c>
+      <c r="AC4" s="36">
+        <v>18</v>
+      </c>
+      <c r="AD4" s="36">
+        <v>19</v>
+      </c>
+      <c r="AE4" s="36">
+        <v>20</v>
+      </c>
+      <c r="AF4" s="36">
+        <v>21</v>
+      </c>
+      <c r="AG4" s="36">
+        <v>22</v>
+      </c>
+      <c r="AH4" s="36">
+        <v>23</v>
+      </c>
+      <c r="AI4" s="36">
+        <v>24</v>
+      </c>
+      <c r="AJ4" s="37">
+        <v>25</v>
+      </c>
+      <c r="AK4" s="4"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>66</v>
@@ -885,8 +1181,53 @@
         <v>7</v>
       </c>
       <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="29">
+        <f>MEDIAN(L5:AJ5)</f>
+        <v>1.0920138888888889E-2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>89</v>
+      </c>
+      <c r="L5" s="29">
+        <v>2.7546296296296294E-3</v>
+      </c>
+      <c r="M5" s="30">
+        <v>5.0462962962962961E-3</v>
+      </c>
+      <c r="N5" s="30">
+        <v>9.4444444444444445E-3</v>
+      </c>
+      <c r="O5" s="30">
+        <v>1.2395833333333335E-2</v>
+      </c>
+      <c r="P5" s="30">
+        <v>1.4074074074074074E-2</v>
+      </c>
+      <c r="Q5" s="30">
+        <v>0.99434027777777778</v>
+      </c>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+      <c r="AC5" s="31"/>
+      <c r="AD5" s="31"/>
+      <c r="AE5" s="31"/>
+      <c r="AF5" s="31"/>
+      <c r="AG5" s="31"/>
+      <c r="AH5" s="31"/>
+      <c r="AI5" s="31"/>
+      <c r="AJ5" s="33"/>
+      <c r="AK5" s="4"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>67</v>
@@ -912,8 +1253,53 @@
         <v>9</v>
       </c>
       <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="29">
+        <f>MEDIAN(L6:AJ6)</f>
+        <v>1.3344907407407408E-2</v>
+      </c>
+      <c r="K6" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="29">
+        <v>1.0902777777777777E-2</v>
+      </c>
+      <c r="M6" s="30">
+        <v>1.1238425925925928E-2</v>
+      </c>
+      <c r="N6" s="30">
+        <v>1.2222222222222223E-2</v>
+      </c>
+      <c r="O6" s="30">
+        <v>1.4467592592592593E-2</v>
+      </c>
+      <c r="P6" s="30">
+        <v>2.8171296296296302E-2</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>0.98700231481481471</v>
+      </c>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
+      <c r="T6" s="31"/>
+      <c r="U6" s="31"/>
+      <c r="V6" s="31"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="31"/>
+      <c r="Y6" s="31"/>
+      <c r="Z6" s="31"/>
+      <c r="AA6" s="31"/>
+      <c r="AB6" s="31"/>
+      <c r="AC6" s="31"/>
+      <c r="AD6" s="31"/>
+      <c r="AE6" s="31"/>
+      <c r="AF6" s="31"/>
+      <c r="AG6" s="31"/>
+      <c r="AH6" s="31"/>
+      <c r="AI6" s="31"/>
+      <c r="AJ6" s="33"/>
+      <c r="AK6" s="4"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>68</v>
@@ -939,8 +1325,53 @@
         <v>7</v>
       </c>
       <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="29">
+        <f>MEDIAN(L7:AJ7)</f>
+        <v>1.7071759259259259E-2</v>
+      </c>
+      <c r="K7" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="29">
+        <v>3.5648148148148154E-3</v>
+      </c>
+      <c r="M7" s="30">
+        <v>1.2627314814814815E-2</v>
+      </c>
+      <c r="N7" s="30">
+        <v>1.3842592592592594E-2</v>
+      </c>
+      <c r="O7" s="30">
+        <v>2.0300925925925927E-2</v>
+      </c>
+      <c r="P7" s="30">
+        <v>2.2453703703703708E-2</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>2.9027777777777777E-2</v>
+      </c>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="31"/>
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="31"/>
+      <c r="AB7" s="31"/>
+      <c r="AC7" s="31"/>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="31"/>
+      <c r="AF7" s="31"/>
+      <c r="AG7" s="31"/>
+      <c r="AH7" s="31"/>
+      <c r="AI7" s="31"/>
+      <c r="AJ7" s="33"/>
+      <c r="AK7" s="4"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>69</v>
@@ -966,8 +1397,53 @@
         <v>70</v>
       </c>
       <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="29">
+        <f>MEDIAN(L8:AJ8)</f>
+        <v>2.2795138888888886E-2</v>
+      </c>
+      <c r="K8" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="29">
+        <v>7.5231481481481477E-3</v>
+      </c>
+      <c r="M8" s="30">
+        <v>1.3275462962962963E-2</v>
+      </c>
+      <c r="N8" s="30">
+        <v>1.4236111111111111E-2</v>
+      </c>
+      <c r="O8" s="30">
+        <v>3.1354166666666662E-2</v>
+      </c>
+      <c r="P8" s="30">
+        <v>3.9803240740740743E-2</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>7.9502314814814817E-2</v>
+      </c>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="31"/>
+      <c r="AB8" s="31"/>
+      <c r="AC8" s="31"/>
+      <c r="AD8" s="31"/>
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="31"/>
+      <c r="AG8" s="31"/>
+      <c r="AH8" s="31"/>
+      <c r="AI8" s="31"/>
+      <c r="AJ8" s="33"/>
+      <c r="AK8" s="4"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>71</v>
@@ -993,8 +1469,53 @@
         <v>9</v>
       </c>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="29">
+        <f>MEDIAN(L9:AJ9)</f>
+        <v>2.5283564814814811E-2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="29">
+        <v>4.6412037037037038E-3</v>
+      </c>
+      <c r="M9" s="30">
+        <v>8.1365740740740738E-3</v>
+      </c>
+      <c r="N9" s="30">
+        <v>2.2349537037037032E-2</v>
+      </c>
+      <c r="O9" s="30">
+        <v>2.8217592592592589E-2</v>
+      </c>
+      <c r="P9" s="30">
+        <v>3.9421296296296295E-2</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>4.3854166666666666E-2</v>
+      </c>
+      <c r="R9" s="31"/>
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="31"/>
+      <c r="AA9" s="31"/>
+      <c r="AB9" s="31"/>
+      <c r="AC9" s="31"/>
+      <c r="AD9" s="31"/>
+      <c r="AE9" s="31"/>
+      <c r="AF9" s="31"/>
+      <c r="AG9" s="31"/>
+      <c r="AH9" s="31"/>
+      <c r="AI9" s="31"/>
+      <c r="AJ9" s="33"/>
+      <c r="AK9" s="4"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>72</v>
@@ -1020,8 +1541,53 @@
         <v>36</v>
       </c>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="29">
+        <f>MEDIAN(L10:AJ10)</f>
+        <v>3.3159722222222222E-2</v>
+      </c>
+      <c r="K10" t="s">
+        <v>75</v>
+      </c>
+      <c r="L10" s="29">
+        <v>9.3171296296296283E-3</v>
+      </c>
+      <c r="M10" s="30">
+        <v>1.6122685185185184E-2</v>
+      </c>
+      <c r="N10" s="30">
+        <v>1.9340277777777779E-2</v>
+      </c>
+      <c r="O10" s="30">
+        <v>4.6979166666666662E-2</v>
+      </c>
+      <c r="P10" s="30">
+        <v>5.2094907407407409E-2</v>
+      </c>
+      <c r="Q10" s="30">
+        <v>0.32503472222222224</v>
+      </c>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AC10" s="31"/>
+      <c r="AD10" s="31"/>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+      <c r="AG10" s="31"/>
+      <c r="AH10" s="31"/>
+      <c r="AI10" s="31"/>
+      <c r="AJ10" s="33"/>
+      <c r="AK10" s="4"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>47</v>
@@ -1039,8 +1605,53 @@
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="29">
+        <f>MEDIAN(L11:AJ11)</f>
+        <v>3.5549768518518515E-2</v>
+      </c>
+      <c r="K11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L11" s="29">
+        <v>1.0046296296296296E-2</v>
+      </c>
+      <c r="M11" s="30">
+        <v>1.2511574074074073E-2</v>
+      </c>
+      <c r="N11" s="30">
+        <v>2.7835648148148151E-2</v>
+      </c>
+      <c r="O11" s="30">
+        <v>4.3263888888888886E-2</v>
+      </c>
+      <c r="P11" s="30">
+        <v>4.3449074074074077E-2</v>
+      </c>
+      <c r="Q11" s="30">
+        <v>6.2546296296296294E-2</v>
+      </c>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
+      <c r="T11" s="31"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="31"/>
+      <c r="Z11" s="31"/>
+      <c r="AA11" s="31"/>
+      <c r="AB11" s="31"/>
+      <c r="AC11" s="31"/>
+      <c r="AD11" s="31"/>
+      <c r="AE11" s="31"/>
+      <c r="AF11" s="31"/>
+      <c r="AG11" s="31"/>
+      <c r="AH11" s="31"/>
+      <c r="AI11" s="31"/>
+      <c r="AJ11" s="33"/>
+      <c r="AK11" s="4"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>48</v>
@@ -1058,8 +1669,53 @@
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="29">
+        <f>MEDIAN(L12:AJ12)</f>
+        <v>4.3657407407407409E-2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" s="29">
+        <v>1.5347222222222222E-2</v>
+      </c>
+      <c r="M12" s="30">
+        <v>2.6550925925925926E-2</v>
+      </c>
+      <c r="N12" s="30">
+        <v>3.8935185185185191E-2</v>
+      </c>
+      <c r="O12" s="30">
+        <v>4.8379629629629627E-2</v>
+      </c>
+      <c r="P12" s="30">
+        <v>6.0162037037037042E-2</v>
+      </c>
+      <c r="Q12" s="30">
+        <v>0.4409953703703704</v>
+      </c>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="31"/>
+      <c r="Y12" s="31"/>
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="31"/>
+      <c r="AB12" s="31"/>
+      <c r="AC12" s="31"/>
+      <c r="AD12" s="31"/>
+      <c r="AE12" s="31"/>
+      <c r="AF12" s="31"/>
+      <c r="AG12" s="31"/>
+      <c r="AH12" s="31"/>
+      <c r="AI12" s="31"/>
+      <c r="AJ12" s="33"/>
+      <c r="AK12" s="4"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>49</v>
@@ -1077,8 +1733,53 @@
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="29">
+        <f>MEDIAN(L13:AJ13)</f>
+        <v>4.8553240740740744E-2</v>
+      </c>
+      <c r="K13" t="s">
+        <v>92</v>
+      </c>
+      <c r="L13" s="29">
+        <v>8.7037037037037031E-3</v>
+      </c>
+      <c r="M13" s="30">
+        <v>2.0254629629629629E-2</v>
+      </c>
+      <c r="N13" s="30">
+        <v>3.6423611111111115E-2</v>
+      </c>
+      <c r="O13" s="30">
+        <v>6.0682870370370373E-2</v>
+      </c>
+      <c r="P13" s="30">
+        <v>0.1423611111111111</v>
+      </c>
+      <c r="Q13" s="32">
+        <v>0.57884259259259252</v>
+      </c>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="31"/>
+      <c r="AB13" s="31"/>
+      <c r="AC13" s="31"/>
+      <c r="AD13" s="31"/>
+      <c r="AE13" s="31"/>
+      <c r="AF13" s="31"/>
+      <c r="AG13" s="31"/>
+      <c r="AH13" s="31"/>
+      <c r="AI13" s="31"/>
+      <c r="AJ13" s="33"/>
+      <c r="AK13" s="4"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>50</v>
@@ -1096,8 +1797,53 @@
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="29">
+        <f>MEDIAN(L14:AJ14)</f>
+        <v>5.1701388888888894E-2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>83</v>
+      </c>
+      <c r="L14" s="29">
+        <v>2.4432870370370369E-2</v>
+      </c>
+      <c r="M14" s="30">
+        <v>2.5590277777777778E-2</v>
+      </c>
+      <c r="N14" s="30">
+        <v>3.3993055555555561E-2</v>
+      </c>
+      <c r="O14" s="30">
+        <v>6.9409722222222234E-2</v>
+      </c>
+      <c r="P14" s="30">
+        <v>0.1012037037037037</v>
+      </c>
+      <c r="Q14" s="30">
+        <v>0.80806712962962957</v>
+      </c>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
+      <c r="AB14" s="31"/>
+      <c r="AC14" s="31"/>
+      <c r="AD14" s="31"/>
+      <c r="AE14" s="31"/>
+      <c r="AF14" s="31"/>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="31"/>
+      <c r="AI14" s="31"/>
+      <c r="AJ14" s="33"/>
+      <c r="AK14" s="4"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>51</v>
@@ -1115,8 +1861,53 @@
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="29">
+        <f>MEDIAN(L15:AJ15)</f>
+        <v>6.5642361111111103E-2</v>
+      </c>
+      <c r="K15" t="s">
+        <v>74</v>
+      </c>
+      <c r="L15" s="29">
+        <v>1.6076388888888887E-2</v>
+      </c>
+      <c r="M15" s="30">
+        <v>4.5983796296296293E-2</v>
+      </c>
+      <c r="N15" s="30">
+        <v>5.0972222222222224E-2</v>
+      </c>
+      <c r="O15" s="30">
+        <v>8.0312499999999995E-2</v>
+      </c>
+      <c r="P15" s="30">
+        <v>0.10246527777777777</v>
+      </c>
+      <c r="Q15" s="30">
+        <v>0.11885416666666666</v>
+      </c>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
+      <c r="X15" s="31"/>
+      <c r="Y15" s="31"/>
+      <c r="Z15" s="31"/>
+      <c r="AA15" s="31"/>
+      <c r="AB15" s="31"/>
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="31"/>
+      <c r="AE15" s="31"/>
+      <c r="AF15" s="31"/>
+      <c r="AG15" s="31"/>
+      <c r="AH15" s="31"/>
+      <c r="AI15" s="31"/>
+      <c r="AJ15" s="33"/>
+      <c r="AK15" s="4"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>52</v>
@@ -1134,8 +1925,53 @@
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="29">
+        <f>MEDIAN(L16:AJ16)</f>
+        <v>6.9328703703703698E-2</v>
+      </c>
+      <c r="K16" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" s="29">
+        <v>1.4293981481481482E-2</v>
+      </c>
+      <c r="M16" s="30">
+        <v>5.0601851851851849E-2</v>
+      </c>
+      <c r="N16" s="30">
+        <v>5.5208333333333331E-2</v>
+      </c>
+      <c r="O16" s="30">
+        <v>8.3449074074074078E-2</v>
+      </c>
+      <c r="P16" s="30">
+        <v>0.92543981481481474</v>
+      </c>
+      <c r="Q16" s="30">
+        <v>1.8910995370370369</v>
+      </c>
+      <c r="R16" s="31"/>
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="31"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="31"/>
+      <c r="AE16" s="31"/>
+      <c r="AF16" s="31"/>
+      <c r="AG16" s="31"/>
+      <c r="AH16" s="31"/>
+      <c r="AI16" s="31"/>
+      <c r="AJ16" s="33"/>
+      <c r="AK16" s="4"/>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>53</v>
@@ -1153,8 +1989,53 @@
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="29">
+        <f>MEDIAN(L17:AJ17)</f>
+        <v>0.10067708333333333</v>
+      </c>
+      <c r="K17" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="29">
+        <v>5.6550925925925921E-2</v>
+      </c>
+      <c r="M17" s="30">
+        <v>5.7037037037037032E-2</v>
+      </c>
+      <c r="N17" s="30">
+        <v>0.10049768518518519</v>
+      </c>
+      <c r="O17" s="30">
+        <v>0.10085648148148148</v>
+      </c>
+      <c r="P17" s="30">
+        <v>0.5876851851851852</v>
+      </c>
+      <c r="Q17" s="30">
+        <v>0.84295138888888888</v>
+      </c>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="31"/>
+      <c r="Y17" s="31"/>
+      <c r="Z17" s="31"/>
+      <c r="AA17" s="31"/>
+      <c r="AB17" s="31"/>
+      <c r="AC17" s="31"/>
+      <c r="AD17" s="31"/>
+      <c r="AE17" s="31"/>
+      <c r="AF17" s="31"/>
+      <c r="AG17" s="31"/>
+      <c r="AH17" s="31"/>
+      <c r="AI17" s="31"/>
+      <c r="AJ17" s="33"/>
+      <c r="AK17" s="4"/>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>54</v>
@@ -1172,8 +2053,53 @@
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="29">
+        <f>MEDIAN(L18:AJ18)</f>
+        <v>0.17217592592592593</v>
+      </c>
+      <c r="K18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L18" s="29">
+        <v>1.4293981481481482E-2</v>
+      </c>
+      <c r="M18" s="30">
+        <v>1.90625E-2</v>
+      </c>
+      <c r="N18" s="30">
+        <v>3.4374999999999996E-2</v>
+      </c>
+      <c r="O18" s="30">
+        <v>0.30997685185185186</v>
+      </c>
+      <c r="P18" s="30">
+        <v>0.33309027777777778</v>
+      </c>
+      <c r="Q18" s="30">
+        <v>0.36160879629629633</v>
+      </c>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
+      <c r="AG18" s="31"/>
+      <c r="AH18" s="31"/>
+      <c r="AI18" s="31"/>
+      <c r="AJ18" s="33"/>
+      <c r="AK18" s="4"/>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>55</v>
@@ -1191,8 +2117,53 @@
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="29">
+        <f>MEDIAN(L19:AJ19)</f>
+        <v>0.20630208333333333</v>
+      </c>
+      <c r="K19" t="s">
+        <v>85</v>
+      </c>
+      <c r="L19" s="29">
+        <v>2.146990740740741E-2</v>
+      </c>
+      <c r="M19" s="30">
+        <v>3.7986111111111116E-2</v>
+      </c>
+      <c r="N19" s="30">
+        <v>0.18174768518518516</v>
+      </c>
+      <c r="O19" s="30">
+        <v>0.2308564814814815</v>
+      </c>
+      <c r="P19" s="30">
+        <v>0.5154050925925926</v>
+      </c>
+      <c r="Q19" s="32">
+        <v>0.90851851851851861</v>
+      </c>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="31"/>
+      <c r="Z19" s="31"/>
+      <c r="AA19" s="31"/>
+      <c r="AB19" s="31"/>
+      <c r="AC19" s="31"/>
+      <c r="AD19" s="31"/>
+      <c r="AE19" s="31"/>
+      <c r="AF19" s="31"/>
+      <c r="AG19" s="31"/>
+      <c r="AH19" s="31"/>
+      <c r="AI19" s="31"/>
+      <c r="AJ19" s="33"/>
+      <c r="AK19" s="4"/>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>56</v>
@@ -1210,8 +2181,53 @@
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="29">
+        <f>MEDIAN(L20:AJ20)</f>
+        <v>0.26016203703703705</v>
+      </c>
+      <c r="K20" t="s">
+        <v>90</v>
+      </c>
+      <c r="L20" s="29">
+        <v>1.8356481481481481E-2</v>
+      </c>
+      <c r="M20" s="30">
+        <v>2.5057870370370373E-2</v>
+      </c>
+      <c r="N20" s="30">
+        <v>2.5092592592592593E-2</v>
+      </c>
+      <c r="O20" s="30">
+        <v>0.49523148148148149</v>
+      </c>
+      <c r="P20" s="30">
+        <v>0.5299652777777778</v>
+      </c>
+      <c r="Q20" s="30">
+        <v>0.55078703703703702</v>
+      </c>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="31"/>
+      <c r="AB20" s="31"/>
+      <c r="AC20" s="31"/>
+      <c r="AD20" s="31"/>
+      <c r="AE20" s="31"/>
+      <c r="AF20" s="31"/>
+      <c r="AG20" s="31"/>
+      <c r="AH20" s="31"/>
+      <c r="AI20" s="31"/>
+      <c r="AJ20" s="33"/>
+      <c r="AK20" s="4"/>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>57</v>
@@ -1229,8 +2245,53 @@
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="29">
+        <f>MEDIAN(L21:AJ21)</f>
+        <v>0.29783564814814811</v>
+      </c>
+      <c r="K21" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="29">
+        <v>2.9513888888888892E-2</v>
+      </c>
+      <c r="M21" s="30">
+        <v>0.27880787037037036</v>
+      </c>
+      <c r="N21" s="30">
+        <v>0.28791666666666665</v>
+      </c>
+      <c r="O21" s="30">
+        <v>0.30775462962962963</v>
+      </c>
+      <c r="P21" s="30">
+        <v>0.34497685185185184</v>
+      </c>
+      <c r="Q21" s="30">
+        <v>0.78767361111111101</v>
+      </c>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="31"/>
+      <c r="AB21" s="31"/>
+      <c r="AC21" s="31"/>
+      <c r="AD21" s="31"/>
+      <c r="AE21" s="31"/>
+      <c r="AF21" s="31"/>
+      <c r="AG21" s="31"/>
+      <c r="AH21" s="31"/>
+      <c r="AI21" s="31"/>
+      <c r="AJ21" s="33"/>
+      <c r="AK21" s="4"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>58</v>
@@ -1248,8 +2309,53 @@
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="29">
+        <f>MEDIAN(L22:AJ22)</f>
+        <v>0.30796296296296299</v>
+      </c>
+      <c r="K22" t="s">
+        <v>95</v>
+      </c>
+      <c r="L22" s="29">
+        <v>6.1041666666666661E-2</v>
+      </c>
+      <c r="M22" s="30">
+        <v>0.13167824074074075</v>
+      </c>
+      <c r="N22" s="30">
+        <v>0.18990740740740741</v>
+      </c>
+      <c r="O22" s="30">
+        <v>0.42601851851851852</v>
+      </c>
+      <c r="P22" s="30">
+        <v>0.54934027777777772</v>
+      </c>
+      <c r="Q22" s="32">
+        <v>0.80325231481481485</v>
+      </c>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="31"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31"/>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="31"/>
+      <c r="AE22" s="31"/>
+      <c r="AF22" s="31"/>
+      <c r="AG22" s="31"/>
+      <c r="AH22" s="31"/>
+      <c r="AI22" s="31"/>
+      <c r="AJ22" s="33"/>
+      <c r="AK22" s="4"/>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>59</v>
@@ -1267,8 +2373,53 @@
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="29">
+        <f>MEDIAN(L23:AJ23)</f>
+        <v>0.32494212962962965</v>
+      </c>
+      <c r="K23" t="s">
+        <v>91</v>
+      </c>
+      <c r="L23" s="29">
+        <v>0.29381944444444447</v>
+      </c>
+      <c r="M23" s="30">
+        <v>0.31736111111111115</v>
+      </c>
+      <c r="N23" s="30">
+        <v>0.32460648148148147</v>
+      </c>
+      <c r="O23" s="30">
+        <v>0.32527777777777778</v>
+      </c>
+      <c r="P23" s="30">
+        <v>0.35981481481481481</v>
+      </c>
+      <c r="Q23" s="30">
+        <v>1.2983449074074074</v>
+      </c>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="31"/>
+      <c r="AA23" s="31"/>
+      <c r="AB23" s="31"/>
+      <c r="AC23" s="31"/>
+      <c r="AD23" s="31"/>
+      <c r="AE23" s="31"/>
+      <c r="AF23" s="31"/>
+      <c r="AG23" s="31"/>
+      <c r="AH23" s="31"/>
+      <c r="AI23" s="31"/>
+      <c r="AJ23" s="33"/>
+      <c r="AK23" s="4"/>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
         <v>60</v>
@@ -1286,8 +2437,53 @@
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="29">
+        <f>MEDIAN(L24:AJ24)</f>
+        <v>0.3666956018518519</v>
+      </c>
+      <c r="K24" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="29">
+        <v>0.31263888888888886</v>
+      </c>
+      <c r="M24" s="30">
+        <v>0.31983796296296296</v>
+      </c>
+      <c r="N24" s="30">
+        <v>0.35513888888888889</v>
+      </c>
+      <c r="O24" s="30">
+        <v>0.37825231481481486</v>
+      </c>
+      <c r="P24" s="30">
+        <v>0.50443287037037032</v>
+      </c>
+      <c r="Q24" s="30">
+        <v>0.54858796296296297</v>
+      </c>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
+      <c r="T24" s="31"/>
+      <c r="U24" s="31"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="31"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="31"/>
+      <c r="AE24" s="31"/>
+      <c r="AF24" s="31"/>
+      <c r="AG24" s="31"/>
+      <c r="AH24" s="31"/>
+      <c r="AI24" s="31"/>
+      <c r="AJ24" s="33"/>
+      <c r="AK24" s="4"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>61</v>
@@ -1305,8 +2501,53 @@
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="29">
+        <f>MEDIAN(L25:AJ25)</f>
+        <v>0.39312499999999995</v>
+      </c>
+      <c r="K25" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25" s="29">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="M25" s="30">
+        <v>0.25746527777777778</v>
+      </c>
+      <c r="N25" s="30">
+        <v>0.38452546296296292</v>
+      </c>
+      <c r="O25" s="30">
+        <v>0.40172453703703703</v>
+      </c>
+      <c r="P25" s="30">
+        <v>0.48754629629629626</v>
+      </c>
+      <c r="Q25" s="30">
+        <v>0.65498842592592588</v>
+      </c>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="31"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="31"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31"/>
+      <c r="AG25" s="31"/>
+      <c r="AH25" s="31"/>
+      <c r="AI25" s="31"/>
+      <c r="AJ25" s="33"/>
+      <c r="AK25" s="4"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>62</v>
@@ -1324,8 +2565,53 @@
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="29">
+        <f>MEDIAN(L26:AJ26)</f>
+        <v>0.39505787037037038</v>
+      </c>
+      <c r="K26" t="s">
+        <v>87</v>
+      </c>
+      <c r="L26" s="29">
+        <v>3.7245370370370366E-2</v>
+      </c>
+      <c r="M26" s="30">
+        <v>0.22336805555555553</v>
+      </c>
+      <c r="N26" s="30">
+        <v>0.30394675925925924</v>
+      </c>
+      <c r="O26" s="30">
+        <v>0.48616898148148152</v>
+      </c>
+      <c r="P26" s="30">
+        <v>0.88638888888888889</v>
+      </c>
+      <c r="Q26" s="30">
+        <v>1.1883796296296296</v>
+      </c>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
+      <c r="T26" s="31"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="31"/>
+      <c r="W26" s="31"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="31"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="31"/>
+      <c r="AC26" s="31"/>
+      <c r="AD26" s="31"/>
+      <c r="AE26" s="31"/>
+      <c r="AF26" s="31"/>
+      <c r="AG26" s="31"/>
+      <c r="AH26" s="31"/>
+      <c r="AI26" s="31"/>
+      <c r="AJ26" s="33"/>
+      <c r="AK26" s="4"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>63</v>
@@ -1343,8 +2629,35 @@
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="31"/>
+      <c r="Z27" s="31"/>
+      <c r="AA27" s="31"/>
+      <c r="AB27" s="31"/>
+      <c r="AC27" s="31"/>
+      <c r="AD27" s="31"/>
+      <c r="AE27" s="31"/>
+      <c r="AF27" s="31"/>
+      <c r="AG27" s="31"/>
+      <c r="AH27" s="31"/>
+      <c r="AI27" s="31"/>
+      <c r="AJ27" s="33"/>
+      <c r="AK27" s="4"/>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>64</v>
@@ -1362,8 +2675,35 @@
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
+      <c r="P28" s="31"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="31"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="31"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
+      <c r="X28" s="31"/>
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="31"/>
+      <c r="AC28" s="31"/>
+      <c r="AD28" s="31"/>
+      <c r="AE28" s="31"/>
+      <c r="AF28" s="31"/>
+      <c r="AG28" s="31"/>
+      <c r="AH28" s="31"/>
+      <c r="AI28" s="31"/>
+      <c r="AJ28" s="33"/>
+      <c r="AK28" s="4"/>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>65</v>
@@ -1381,74 +2721,172 @@
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
+      <c r="X29" s="31"/>
+      <c r="Y29" s="31"/>
+      <c r="Z29" s="31"/>
+      <c r="AA29" s="31"/>
+      <c r="AB29" s="31"/>
+      <c r="AC29" s="31"/>
+      <c r="AD29" s="31"/>
+      <c r="AE29" s="31"/>
+      <c r="AF29" s="31"/>
+      <c r="AG29" s="31"/>
+      <c r="AH29" s="31"/>
+      <c r="AI29" s="31"/>
+      <c r="AJ29" s="33"/>
+      <c r="AK29" s="4"/>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="40"/>
       <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D32" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="23">
-        <f>MEDIAN(E5:E29)</f>
-        <v>1.7071759259259259E-2</v>
-      </c>
+      <c r="J30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="31"/>
+      <c r="AA30" s="31"/>
+      <c r="AB30" s="31"/>
+      <c r="AC30" s="31"/>
+      <c r="AD30" s="31"/>
+      <c r="AE30" s="31"/>
+      <c r="AF30" s="31"/>
+      <c r="AG30" s="31"/>
+      <c r="AH30" s="31"/>
+      <c r="AI30" s="31"/>
+      <c r="AJ30" s="33"/>
+      <c r="AK30" s="4"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A31" s="41"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="AK31" s="4"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="D32" s="24"/>
+      <c r="E32" s="23"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="24"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="4"/>
+      <c r="AK32" s="4"/>
+    </row>
+    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="I33" s="4"/>
+      <c r="AK33" s="4"/>
+    </row>
+    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="I34" s="4"/>
+      <c r="AK34" s="4"/>
+    </row>
+    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="I35" s="4"/>
+      <c r="AK35" s="4"/>
+    </row>
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="E36" s="25"/>
+      <c r="I36" s="4"/>
+      <c r="AK36" s="4"/>
+    </row>
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E37" s="25"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="4"/>
+      <c r="AK37" s="4"/>
+    </row>
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E38" s="25"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I38" s="4"/>
+      <c r="AK38" s="4"/>
+    </row>
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E39" s="25"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I39" s="4"/>
+      <c r="AK39" s="4"/>
+    </row>
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E40" s="25"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E41" s="25"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
       <c r="E42" s="25"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E43" s="25"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E44" s="26"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="E43" s="26"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B45" s="25"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="4"/>
     </row>
   </sheetData>
+  <sortState ref="J5:Q26">
+    <sortCondition ref="J5:J26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated viz to include median times on the webpage.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -234,75 +234,6 @@
   </si>
   <si>
     <t>Day 6: Universal Orbit Map</t>
-  </si>
-  <si>
-    <t>Participant</t>
-  </si>
-  <si>
-    <t>Andrew Chang</t>
-  </si>
-  <si>
-    <t>Sam Holton</t>
-  </si>
-  <si>
-    <t>Elise Thorsen</t>
-  </si>
-  <si>
-    <t>Michael Herms</t>
-  </si>
-  <si>
-    <t>Taybin Rutkin</t>
-  </si>
-  <si>
-    <t>Shauna Revay</t>
-  </si>
-  <si>
-    <t>Eric Hughes</t>
-  </si>
-  <si>
-    <t>Matt Boehm</t>
-  </si>
-  <si>
-    <t>Lara Dedic</t>
-  </si>
-  <si>
-    <t>Rebecca Matous</t>
-  </si>
-  <si>
-    <t>Greg Fuller</t>
-  </si>
-  <si>
-    <t>Bradley Welsh</t>
-  </si>
-  <si>
-    <t>Jesse Florig</t>
-  </si>
-  <si>
-    <t>Robert Roger</t>
-  </si>
-  <si>
-    <t>Christopher Tibbetts</t>
-  </si>
-  <si>
-    <t>Nathan Shirley</t>
-  </si>
-  <si>
-    <t>Quintin DeGroot</t>
-  </si>
-  <si>
-    <t>Richard Bradley</t>
-  </si>
-  <si>
-    <t>Jonathan Skeate</t>
-  </si>
-  <si>
-    <t>Alan Carvajal</t>
-  </si>
-  <si>
-    <t>Brian Uri</t>
-  </si>
-  <si>
-    <t>Jeremy Glesner</t>
   </si>
 </sst>
 </file>
@@ -378,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -479,48 +410,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -582,19 +476,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -906,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK52"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,12 +799,10 @@
     <col min="2" max="2" width="42.5703125" customWidth="1"/>
     <col min="3" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="6.85546875" customWidth="1"/>
-    <col min="10" max="10" width="7.7109375" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="46" width="8" customWidth="1"/>
+    <col min="10" max="18" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -933,36 +812,8 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="8"/>
       <c r="C2" s="13"/>
@@ -976,36 +827,8 @@
       </c>
       <c r="H2" s="27"/>
       <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="4"/>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="4"/>
-      <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4"/>
-      <c r="AK2" s="4"/>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="18"/>
       <c r="C3" s="10"/>
@@ -1019,36 +842,8 @@
         <v>17</v>
       </c>
       <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -1072,90 +867,8 @@
         <v>46</v>
       </c>
       <c r="I4" s="4"/>
-      <c r="J4" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="L4" s="36">
-        <v>1</v>
-      </c>
-      <c r="M4" s="36">
-        <v>2</v>
-      </c>
-      <c r="N4" s="36">
-        <v>3</v>
-      </c>
-      <c r="O4" s="36">
-        <v>4</v>
-      </c>
-      <c r="P4" s="36">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="36">
-        <v>6</v>
-      </c>
-      <c r="R4" s="36">
-        <v>7</v>
-      </c>
-      <c r="S4" s="36">
-        <v>8</v>
-      </c>
-      <c r="T4" s="36">
-        <v>9</v>
-      </c>
-      <c r="U4" s="36">
-        <v>10</v>
-      </c>
-      <c r="V4" s="36">
-        <v>11</v>
-      </c>
-      <c r="W4" s="36">
-        <v>12</v>
-      </c>
-      <c r="X4" s="36">
-        <v>13</v>
-      </c>
-      <c r="Y4" s="36">
-        <v>14</v>
-      </c>
-      <c r="Z4" s="36">
-        <v>15</v>
-      </c>
-      <c r="AA4" s="36">
-        <v>16</v>
-      </c>
-      <c r="AB4" s="36">
-        <v>17</v>
-      </c>
-      <c r="AC4" s="36">
-        <v>18</v>
-      </c>
-      <c r="AD4" s="36">
-        <v>19</v>
-      </c>
-      <c r="AE4" s="36">
-        <v>20</v>
-      </c>
-      <c r="AF4" s="36">
-        <v>21</v>
-      </c>
-      <c r="AG4" s="36">
-        <v>22</v>
-      </c>
-      <c r="AH4" s="36">
-        <v>23</v>
-      </c>
-      <c r="AI4" s="36">
-        <v>24</v>
-      </c>
-      <c r="AJ4" s="37">
-        <v>25</v>
-      </c>
-      <c r="AK4" s="4"/>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>66</v>
@@ -1181,53 +894,8 @@
         <v>7</v>
       </c>
       <c r="I5" s="4"/>
-      <c r="J5" s="29">
-        <f>MEDIAN(L5:AJ5)</f>
-        <v>1.0920138888888889E-2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>89</v>
-      </c>
-      <c r="L5" s="29">
-        <v>2.7546296296296294E-3</v>
-      </c>
-      <c r="M5" s="30">
-        <v>5.0462962962962961E-3</v>
-      </c>
-      <c r="N5" s="30">
-        <v>9.4444444444444445E-3</v>
-      </c>
-      <c r="O5" s="30">
-        <v>1.2395833333333335E-2</v>
-      </c>
-      <c r="P5" s="30">
-        <v>1.4074074074074074E-2</v>
-      </c>
-      <c r="Q5" s="30">
-        <v>0.99434027777777778</v>
-      </c>
-      <c r="R5" s="31"/>
-      <c r="S5" s="31"/>
-      <c r="T5" s="31"/>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31"/>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="31"/>
-      <c r="AD5" s="31"/>
-      <c r="AE5" s="31"/>
-      <c r="AF5" s="31"/>
-      <c r="AG5" s="31"/>
-      <c r="AH5" s="31"/>
-      <c r="AI5" s="31"/>
-      <c r="AJ5" s="33"/>
-      <c r="AK5" s="4"/>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>67</v>
@@ -1253,53 +921,8 @@
         <v>9</v>
       </c>
       <c r="I6" s="4"/>
-      <c r="J6" s="29">
-        <f>MEDIAN(L6:AJ6)</f>
-        <v>1.3344907407407408E-2</v>
-      </c>
-      <c r="K6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" s="29">
-        <v>1.0902777777777777E-2</v>
-      </c>
-      <c r="M6" s="30">
-        <v>1.1238425925925928E-2</v>
-      </c>
-      <c r="N6" s="30">
-        <v>1.2222222222222223E-2</v>
-      </c>
-      <c r="O6" s="30">
-        <v>1.4467592592592593E-2</v>
-      </c>
-      <c r="P6" s="30">
-        <v>2.8171296296296302E-2</v>
-      </c>
-      <c r="Q6" s="30">
-        <v>0.98700231481481471</v>
-      </c>
-      <c r="R6" s="31"/>
-      <c r="S6" s="31"/>
-      <c r="T6" s="31"/>
-      <c r="U6" s="31"/>
-      <c r="V6" s="31"/>
-      <c r="W6" s="31"/>
-      <c r="X6" s="31"/>
-      <c r="Y6" s="31"/>
-      <c r="Z6" s="31"/>
-      <c r="AA6" s="31"/>
-      <c r="AB6" s="31"/>
-      <c r="AC6" s="31"/>
-      <c r="AD6" s="31"/>
-      <c r="AE6" s="31"/>
-      <c r="AF6" s="31"/>
-      <c r="AG6" s="31"/>
-      <c r="AH6" s="31"/>
-      <c r="AI6" s="31"/>
-      <c r="AJ6" s="33"/>
-      <c r="AK6" s="4"/>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>68</v>
@@ -1325,53 +948,8 @@
         <v>7</v>
       </c>
       <c r="I7" s="4"/>
-      <c r="J7" s="29">
-        <f>MEDIAN(L7:AJ7)</f>
-        <v>1.7071759259259259E-2</v>
-      </c>
-      <c r="K7" t="s">
-        <v>94</v>
-      </c>
-      <c r="L7" s="29">
-        <v>3.5648148148148154E-3</v>
-      </c>
-      <c r="M7" s="30">
-        <v>1.2627314814814815E-2</v>
-      </c>
-      <c r="N7" s="30">
-        <v>1.3842592592592594E-2</v>
-      </c>
-      <c r="O7" s="30">
-        <v>2.0300925925925927E-2</v>
-      </c>
-      <c r="P7" s="30">
-        <v>2.2453703703703708E-2</v>
-      </c>
-      <c r="Q7" s="30">
-        <v>2.9027777777777777E-2</v>
-      </c>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="31"/>
-      <c r="X7" s="31"/>
-      <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="31"/>
-      <c r="AC7" s="31"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="31"/>
-      <c r="AF7" s="31"/>
-      <c r="AG7" s="31"/>
-      <c r="AH7" s="31"/>
-      <c r="AI7" s="31"/>
-      <c r="AJ7" s="33"/>
-      <c r="AK7" s="4"/>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>69</v>
@@ -1397,53 +975,8 @@
         <v>70</v>
       </c>
       <c r="I8" s="4"/>
-      <c r="J8" s="29">
-        <f>MEDIAN(L8:AJ8)</f>
-        <v>2.2795138888888886E-2</v>
-      </c>
-      <c r="K8" t="s">
-        <v>77</v>
-      </c>
-      <c r="L8" s="29">
-        <v>7.5231481481481477E-3</v>
-      </c>
-      <c r="M8" s="30">
-        <v>1.3275462962962963E-2</v>
-      </c>
-      <c r="N8" s="30">
-        <v>1.4236111111111111E-2</v>
-      </c>
-      <c r="O8" s="30">
-        <v>3.1354166666666662E-2</v>
-      </c>
-      <c r="P8" s="30">
-        <v>3.9803240740740743E-2</v>
-      </c>
-      <c r="Q8" s="30">
-        <v>7.9502314814814817E-2</v>
-      </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="31"/>
-      <c r="T8" s="31"/>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="31"/>
-      <c r="X8" s="31"/>
-      <c r="Y8" s="31"/>
-      <c r="Z8" s="31"/>
-      <c r="AA8" s="31"/>
-      <c r="AB8" s="31"/>
-      <c r="AC8" s="31"/>
-      <c r="AD8" s="31"/>
-      <c r="AE8" s="31"/>
-      <c r="AF8" s="31"/>
-      <c r="AG8" s="31"/>
-      <c r="AH8" s="31"/>
-      <c r="AI8" s="31"/>
-      <c r="AJ8" s="33"/>
-      <c r="AK8" s="4"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>71</v>
@@ -1469,53 +1002,8 @@
         <v>9</v>
       </c>
       <c r="I9" s="4"/>
-      <c r="J9" s="29">
-        <f>MEDIAN(L9:AJ9)</f>
-        <v>2.5283564814814811E-2</v>
-      </c>
-      <c r="K9" t="s">
-        <v>84</v>
-      </c>
-      <c r="L9" s="29">
-        <v>4.6412037037037038E-3</v>
-      </c>
-      <c r="M9" s="30">
-        <v>8.1365740740740738E-3</v>
-      </c>
-      <c r="N9" s="30">
-        <v>2.2349537037037032E-2</v>
-      </c>
-      <c r="O9" s="30">
-        <v>2.8217592592592589E-2</v>
-      </c>
-      <c r="P9" s="30">
-        <v>3.9421296296296295E-2</v>
-      </c>
-      <c r="Q9" s="30">
-        <v>4.3854166666666666E-2</v>
-      </c>
-      <c r="R9" s="31"/>
-      <c r="S9" s="31"/>
-      <c r="T9" s="31"/>
-      <c r="U9" s="31"/>
-      <c r="V9" s="31"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="31"/>
-      <c r="Y9" s="31"/>
-      <c r="Z9" s="31"/>
-      <c r="AA9" s="31"/>
-      <c r="AB9" s="31"/>
-      <c r="AC9" s="31"/>
-      <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
-      <c r="AF9" s="31"/>
-      <c r="AG9" s="31"/>
-      <c r="AH9" s="31"/>
-      <c r="AI9" s="31"/>
-      <c r="AJ9" s="33"/>
-      <c r="AK9" s="4"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>72</v>
@@ -1541,53 +1029,8 @@
         <v>36</v>
       </c>
       <c r="I10" s="4"/>
-      <c r="J10" s="29">
-        <f>MEDIAN(L10:AJ10)</f>
-        <v>3.3159722222222222E-2</v>
-      </c>
-      <c r="K10" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="29">
-        <v>9.3171296296296283E-3</v>
-      </c>
-      <c r="M10" s="30">
-        <v>1.6122685185185184E-2</v>
-      </c>
-      <c r="N10" s="30">
-        <v>1.9340277777777779E-2</v>
-      </c>
-      <c r="O10" s="30">
-        <v>4.6979166666666662E-2</v>
-      </c>
-      <c r="P10" s="30">
-        <v>5.2094907407407409E-2</v>
-      </c>
-      <c r="Q10" s="30">
-        <v>0.32503472222222224</v>
-      </c>
-      <c r="R10" s="31"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="31"/>
-      <c r="U10" s="31"/>
-      <c r="V10" s="31"/>
-      <c r="W10" s="31"/>
-      <c r="X10" s="31"/>
-      <c r="Y10" s="31"/>
-      <c r="Z10" s="31"/>
-      <c r="AA10" s="31"/>
-      <c r="AB10" s="31"/>
-      <c r="AC10" s="31"/>
-      <c r="AD10" s="31"/>
-      <c r="AE10" s="31"/>
-      <c r="AF10" s="31"/>
-      <c r="AG10" s="31"/>
-      <c r="AH10" s="31"/>
-      <c r="AI10" s="31"/>
-      <c r="AJ10" s="33"/>
-      <c r="AK10" s="4"/>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>47</v>
@@ -1605,53 +1048,8 @@
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="4"/>
-      <c r="J11" s="29">
-        <f>MEDIAN(L11:AJ11)</f>
-        <v>3.5549768518518515E-2</v>
-      </c>
-      <c r="K11" t="s">
-        <v>93</v>
-      </c>
-      <c r="L11" s="29">
-        <v>1.0046296296296296E-2</v>
-      </c>
-      <c r="M11" s="30">
-        <v>1.2511574074074073E-2</v>
-      </c>
-      <c r="N11" s="30">
-        <v>2.7835648148148151E-2</v>
-      </c>
-      <c r="O11" s="30">
-        <v>4.3263888888888886E-2</v>
-      </c>
-      <c r="P11" s="30">
-        <v>4.3449074074074077E-2</v>
-      </c>
-      <c r="Q11" s="30">
-        <v>6.2546296296296294E-2</v>
-      </c>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="31"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="31"/>
-      <c r="X11" s="31"/>
-      <c r="Y11" s="31"/>
-      <c r="Z11" s="31"/>
-      <c r="AA11" s="31"/>
-      <c r="AB11" s="31"/>
-      <c r="AC11" s="31"/>
-      <c r="AD11" s="31"/>
-      <c r="AE11" s="31"/>
-      <c r="AF11" s="31"/>
-      <c r="AG11" s="31"/>
-      <c r="AH11" s="31"/>
-      <c r="AI11" s="31"/>
-      <c r="AJ11" s="33"/>
-      <c r="AK11" s="4"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>48</v>
@@ -1669,53 +1067,8 @@
       </c>
       <c r="H12" s="16"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="29">
-        <f>MEDIAN(L12:AJ12)</f>
-        <v>4.3657407407407409E-2</v>
-      </c>
-      <c r="K12" t="s">
-        <v>88</v>
-      </c>
-      <c r="L12" s="29">
-        <v>1.5347222222222222E-2</v>
-      </c>
-      <c r="M12" s="30">
-        <v>2.6550925925925926E-2</v>
-      </c>
-      <c r="N12" s="30">
-        <v>3.8935185185185191E-2</v>
-      </c>
-      <c r="O12" s="30">
-        <v>4.8379629629629627E-2</v>
-      </c>
-      <c r="P12" s="30">
-        <v>6.0162037037037042E-2</v>
-      </c>
-      <c r="Q12" s="30">
-        <v>0.4409953703703704</v>
-      </c>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="31"/>
-      <c r="U12" s="31"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="31"/>
-      <c r="X12" s="31"/>
-      <c r="Y12" s="31"/>
-      <c r="Z12" s="31"/>
-      <c r="AA12" s="31"/>
-      <c r="AB12" s="31"/>
-      <c r="AC12" s="31"/>
-      <c r="AD12" s="31"/>
-      <c r="AE12" s="31"/>
-      <c r="AF12" s="31"/>
-      <c r="AG12" s="31"/>
-      <c r="AH12" s="31"/>
-      <c r="AI12" s="31"/>
-      <c r="AJ12" s="33"/>
-      <c r="AK12" s="4"/>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>49</v>
@@ -1733,53 +1086,8 @@
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="4"/>
-      <c r="J13" s="29">
-        <f>MEDIAN(L13:AJ13)</f>
-        <v>4.8553240740740744E-2</v>
-      </c>
-      <c r="K13" t="s">
-        <v>92</v>
-      </c>
-      <c r="L13" s="29">
-        <v>8.7037037037037031E-3</v>
-      </c>
-      <c r="M13" s="30">
-        <v>2.0254629629629629E-2</v>
-      </c>
-      <c r="N13" s="30">
-        <v>3.6423611111111115E-2</v>
-      </c>
-      <c r="O13" s="30">
-        <v>6.0682870370370373E-2</v>
-      </c>
-      <c r="P13" s="30">
-        <v>0.1423611111111111</v>
-      </c>
-      <c r="Q13" s="32">
-        <v>0.57884259259259252</v>
-      </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="31"/>
-      <c r="T13" s="31"/>
-      <c r="U13" s="31"/>
-      <c r="V13" s="31"/>
-      <c r="W13" s="31"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="31"/>
-      <c r="Z13" s="31"/>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="31"/>
-      <c r="AC13" s="31"/>
-      <c r="AD13" s="31"/>
-      <c r="AE13" s="31"/>
-      <c r="AF13" s="31"/>
-      <c r="AG13" s="31"/>
-      <c r="AH13" s="31"/>
-      <c r="AI13" s="31"/>
-      <c r="AJ13" s="33"/>
-      <c r="AK13" s="4"/>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>50</v>
@@ -1797,53 +1105,8 @@
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="4"/>
-      <c r="J14" s="29">
-        <f>MEDIAN(L14:AJ14)</f>
-        <v>5.1701388888888894E-2</v>
-      </c>
-      <c r="K14" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" s="29">
-        <v>2.4432870370370369E-2</v>
-      </c>
-      <c r="M14" s="30">
-        <v>2.5590277777777778E-2</v>
-      </c>
-      <c r="N14" s="30">
-        <v>3.3993055555555561E-2</v>
-      </c>
-      <c r="O14" s="30">
-        <v>6.9409722222222234E-2</v>
-      </c>
-      <c r="P14" s="30">
-        <v>0.1012037037037037</v>
-      </c>
-      <c r="Q14" s="30">
-        <v>0.80806712962962957</v>
-      </c>
-      <c r="R14" s="31"/>
-      <c r="S14" s="31"/>
-      <c r="T14" s="31"/>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="31"/>
-      <c r="X14" s="31"/>
-      <c r="Y14" s="31"/>
-      <c r="Z14" s="31"/>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="31"/>
-      <c r="AC14" s="31"/>
-      <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="31"/>
-      <c r="AI14" s="31"/>
-      <c r="AJ14" s="33"/>
-      <c r="AK14" s="4"/>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>51</v>
@@ -1861,53 +1124,8 @@
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="4"/>
-      <c r="J15" s="29">
-        <f>MEDIAN(L15:AJ15)</f>
-        <v>6.5642361111111103E-2</v>
-      </c>
-      <c r="K15" t="s">
-        <v>74</v>
-      </c>
-      <c r="L15" s="29">
-        <v>1.6076388888888887E-2</v>
-      </c>
-      <c r="M15" s="30">
-        <v>4.5983796296296293E-2</v>
-      </c>
-      <c r="N15" s="30">
-        <v>5.0972222222222224E-2</v>
-      </c>
-      <c r="O15" s="30">
-        <v>8.0312499999999995E-2</v>
-      </c>
-      <c r="P15" s="30">
-        <v>0.10246527777777777</v>
-      </c>
-      <c r="Q15" s="30">
-        <v>0.11885416666666666</v>
-      </c>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
-      <c r="T15" s="31"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
-      <c r="W15" s="31"/>
-      <c r="X15" s="31"/>
-      <c r="Y15" s="31"/>
-      <c r="Z15" s="31"/>
-      <c r="AA15" s="31"/>
-      <c r="AB15" s="31"/>
-      <c r="AC15" s="31"/>
-      <c r="AD15" s="31"/>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31"/>
-      <c r="AG15" s="31"/>
-      <c r="AH15" s="31"/>
-      <c r="AI15" s="31"/>
-      <c r="AJ15" s="33"/>
-      <c r="AK15" s="4"/>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>52</v>
@@ -1925,53 +1143,8 @@
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="29">
-        <f>MEDIAN(L16:AJ16)</f>
-        <v>6.9328703703703698E-2</v>
-      </c>
-      <c r="K16" t="s">
-        <v>80</v>
-      </c>
-      <c r="L16" s="29">
-        <v>1.4293981481481482E-2</v>
-      </c>
-      <c r="M16" s="30">
-        <v>5.0601851851851849E-2</v>
-      </c>
-      <c r="N16" s="30">
-        <v>5.5208333333333331E-2</v>
-      </c>
-      <c r="O16" s="30">
-        <v>8.3449074074074078E-2</v>
-      </c>
-      <c r="P16" s="30">
-        <v>0.92543981481481474</v>
-      </c>
-      <c r="Q16" s="30">
-        <v>1.8910995370370369</v>
-      </c>
-      <c r="R16" s="31"/>
-      <c r="S16" s="31"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="31"/>
-      <c r="X16" s="31"/>
-      <c r="Y16" s="31"/>
-      <c r="Z16" s="31"/>
-      <c r="AA16" s="31"/>
-      <c r="AB16" s="31"/>
-      <c r="AC16" s="31"/>
-      <c r="AD16" s="31"/>
-      <c r="AE16" s="31"/>
-      <c r="AF16" s="31"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="31"/>
-      <c r="AI16" s="31"/>
-      <c r="AJ16" s="33"/>
-      <c r="AK16" s="4"/>
-    </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>53</v>
@@ -1989,53 +1162,8 @@
       </c>
       <c r="H17" s="16"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="29">
-        <f>MEDIAN(L17:AJ17)</f>
-        <v>0.10067708333333333</v>
-      </c>
-      <c r="K17" t="s">
-        <v>86</v>
-      </c>
-      <c r="L17" s="29">
-        <v>5.6550925925925921E-2</v>
-      </c>
-      <c r="M17" s="30">
-        <v>5.7037037037037032E-2</v>
-      </c>
-      <c r="N17" s="30">
-        <v>0.10049768518518519</v>
-      </c>
-      <c r="O17" s="30">
-        <v>0.10085648148148148</v>
-      </c>
-      <c r="P17" s="30">
-        <v>0.5876851851851852</v>
-      </c>
-      <c r="Q17" s="30">
-        <v>0.84295138888888888</v>
-      </c>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="31"/>
-      <c r="Y17" s="31"/>
-      <c r="Z17" s="31"/>
-      <c r="AA17" s="31"/>
-      <c r="AB17" s="31"/>
-      <c r="AC17" s="31"/>
-      <c r="AD17" s="31"/>
-      <c r="AE17" s="31"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="31"/>
-      <c r="AH17" s="31"/>
-      <c r="AI17" s="31"/>
-      <c r="AJ17" s="33"/>
-      <c r="AK17" s="4"/>
-    </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>54</v>
@@ -2053,53 +1181,8 @@
       </c>
       <c r="H18" s="16"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="29">
-        <f>MEDIAN(L18:AJ18)</f>
-        <v>0.17217592592592593</v>
-      </c>
-      <c r="K18" t="s">
-        <v>82</v>
-      </c>
-      <c r="L18" s="29">
-        <v>1.4293981481481482E-2</v>
-      </c>
-      <c r="M18" s="30">
-        <v>1.90625E-2</v>
-      </c>
-      <c r="N18" s="30">
-        <v>3.4374999999999996E-2</v>
-      </c>
-      <c r="O18" s="30">
-        <v>0.30997685185185186</v>
-      </c>
-      <c r="P18" s="30">
-        <v>0.33309027777777778</v>
-      </c>
-      <c r="Q18" s="30">
-        <v>0.36160879629629633</v>
-      </c>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="31"/>
-      <c r="AC18" s="31"/>
-      <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-      <c r="AI18" s="31"/>
-      <c r="AJ18" s="33"/>
-      <c r="AK18" s="4"/>
-    </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>55</v>
@@ -2117,53 +1200,8 @@
       </c>
       <c r="H19" s="16"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="29">
-        <f>MEDIAN(L19:AJ19)</f>
-        <v>0.20630208333333333</v>
-      </c>
-      <c r="K19" t="s">
-        <v>85</v>
-      </c>
-      <c r="L19" s="29">
-        <v>2.146990740740741E-2</v>
-      </c>
-      <c r="M19" s="30">
-        <v>3.7986111111111116E-2</v>
-      </c>
-      <c r="N19" s="30">
-        <v>0.18174768518518516</v>
-      </c>
-      <c r="O19" s="30">
-        <v>0.2308564814814815</v>
-      </c>
-      <c r="P19" s="30">
-        <v>0.5154050925925926</v>
-      </c>
-      <c r="Q19" s="32">
-        <v>0.90851851851851861</v>
-      </c>
-      <c r="R19" s="31"/>
-      <c r="S19" s="31"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="31"/>
-      <c r="X19" s="31"/>
-      <c r="Y19" s="31"/>
-      <c r="Z19" s="31"/>
-      <c r="AA19" s="31"/>
-      <c r="AB19" s="31"/>
-      <c r="AC19" s="31"/>
-      <c r="AD19" s="31"/>
-      <c r="AE19" s="31"/>
-      <c r="AF19" s="31"/>
-      <c r="AG19" s="31"/>
-      <c r="AH19" s="31"/>
-      <c r="AI19" s="31"/>
-      <c r="AJ19" s="33"/>
-      <c r="AK19" s="4"/>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>56</v>
@@ -2181,53 +1219,8 @@
       </c>
       <c r="H20" s="16"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="29">
-        <f>MEDIAN(L20:AJ20)</f>
-        <v>0.26016203703703705</v>
-      </c>
-      <c r="K20" t="s">
-        <v>90</v>
-      </c>
-      <c r="L20" s="29">
-        <v>1.8356481481481481E-2</v>
-      </c>
-      <c r="M20" s="30">
-        <v>2.5057870370370373E-2</v>
-      </c>
-      <c r="N20" s="30">
-        <v>2.5092592592592593E-2</v>
-      </c>
-      <c r="O20" s="30">
-        <v>0.49523148148148149</v>
-      </c>
-      <c r="P20" s="30">
-        <v>0.5299652777777778</v>
-      </c>
-      <c r="Q20" s="30">
-        <v>0.55078703703703702</v>
-      </c>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="31"/>
-      <c r="X20" s="31"/>
-      <c r="Y20" s="31"/>
-      <c r="Z20" s="31"/>
-      <c r="AA20" s="31"/>
-      <c r="AB20" s="31"/>
-      <c r="AC20" s="31"/>
-      <c r="AD20" s="31"/>
-      <c r="AE20" s="31"/>
-      <c r="AF20" s="31"/>
-      <c r="AG20" s="31"/>
-      <c r="AH20" s="31"/>
-      <c r="AI20" s="31"/>
-      <c r="AJ20" s="33"/>
-      <c r="AK20" s="4"/>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>57</v>
@@ -2245,53 +1238,8 @@
       </c>
       <c r="H21" s="16"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="29">
-        <f>MEDIAN(L21:AJ21)</f>
-        <v>0.29783564814814811</v>
-      </c>
-      <c r="K21" t="s">
-        <v>76</v>
-      </c>
-      <c r="L21" s="29">
-        <v>2.9513888888888892E-2</v>
-      </c>
-      <c r="M21" s="30">
-        <v>0.27880787037037036</v>
-      </c>
-      <c r="N21" s="30">
-        <v>0.28791666666666665</v>
-      </c>
-      <c r="O21" s="30">
-        <v>0.30775462962962963</v>
-      </c>
-      <c r="P21" s="30">
-        <v>0.34497685185185184</v>
-      </c>
-      <c r="Q21" s="30">
-        <v>0.78767361111111101</v>
-      </c>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="31"/>
-      <c r="X21" s="31"/>
-      <c r="Y21" s="31"/>
-      <c r="Z21" s="31"/>
-      <c r="AA21" s="31"/>
-      <c r="AB21" s="31"/>
-      <c r="AC21" s="31"/>
-      <c r="AD21" s="31"/>
-      <c r="AE21" s="31"/>
-      <c r="AF21" s="31"/>
-      <c r="AG21" s="31"/>
-      <c r="AH21" s="31"/>
-      <c r="AI21" s="31"/>
-      <c r="AJ21" s="33"/>
-      <c r="AK21" s="4"/>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>58</v>
@@ -2309,53 +1257,8 @@
       </c>
       <c r="H22" s="16"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="29">
-        <f>MEDIAN(L22:AJ22)</f>
-        <v>0.30796296296296299</v>
-      </c>
-      <c r="K22" t="s">
-        <v>95</v>
-      </c>
-      <c r="L22" s="29">
-        <v>6.1041666666666661E-2</v>
-      </c>
-      <c r="M22" s="30">
-        <v>0.13167824074074075</v>
-      </c>
-      <c r="N22" s="30">
-        <v>0.18990740740740741</v>
-      </c>
-      <c r="O22" s="30">
-        <v>0.42601851851851852</v>
-      </c>
-      <c r="P22" s="30">
-        <v>0.54934027777777772</v>
-      </c>
-      <c r="Q22" s="32">
-        <v>0.80325231481481485</v>
-      </c>
-      <c r="R22" s="31"/>
-      <c r="S22" s="31"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="31"/>
-      <c r="Z22" s="31"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="31"/>
-      <c r="AC22" s="31"/>
-      <c r="AD22" s="31"/>
-      <c r="AE22" s="31"/>
-      <c r="AF22" s="31"/>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="31"/>
-      <c r="AI22" s="31"/>
-      <c r="AJ22" s="33"/>
-      <c r="AK22" s="4"/>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>59</v>
@@ -2373,53 +1276,8 @@
       </c>
       <c r="H23" s="16"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="29">
-        <f>MEDIAN(L23:AJ23)</f>
-        <v>0.32494212962962965</v>
-      </c>
-      <c r="K23" t="s">
-        <v>91</v>
-      </c>
-      <c r="L23" s="29">
-        <v>0.29381944444444447</v>
-      </c>
-      <c r="M23" s="30">
-        <v>0.31736111111111115</v>
-      </c>
-      <c r="N23" s="30">
-        <v>0.32460648148148147</v>
-      </c>
-      <c r="O23" s="30">
-        <v>0.32527777777777778</v>
-      </c>
-      <c r="P23" s="30">
-        <v>0.35981481481481481</v>
-      </c>
-      <c r="Q23" s="30">
-        <v>1.2983449074074074</v>
-      </c>
-      <c r="R23" s="31"/>
-      <c r="S23" s="31"/>
-      <c r="T23" s="31"/>
-      <c r="U23" s="31"/>
-      <c r="V23" s="31"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="31"/>
-      <c r="Y23" s="31"/>
-      <c r="Z23" s="31"/>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="31"/>
-      <c r="AC23" s="31"/>
-      <c r="AD23" s="31"/>
-      <c r="AE23" s="31"/>
-      <c r="AF23" s="31"/>
-      <c r="AG23" s="31"/>
-      <c r="AH23" s="31"/>
-      <c r="AI23" s="31"/>
-      <c r="AJ23" s="33"/>
-      <c r="AK23" s="4"/>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
         <v>60</v>
@@ -2437,53 +1295,8 @@
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="4"/>
-      <c r="J24" s="29">
-        <f>MEDIAN(L24:AJ24)</f>
-        <v>0.3666956018518519</v>
-      </c>
-      <c r="K24" t="s">
-        <v>79</v>
-      </c>
-      <c r="L24" s="29">
-        <v>0.31263888888888886</v>
-      </c>
-      <c r="M24" s="30">
-        <v>0.31983796296296296</v>
-      </c>
-      <c r="N24" s="30">
-        <v>0.35513888888888889</v>
-      </c>
-      <c r="O24" s="30">
-        <v>0.37825231481481486</v>
-      </c>
-      <c r="P24" s="30">
-        <v>0.50443287037037032</v>
-      </c>
-      <c r="Q24" s="30">
-        <v>0.54858796296296297</v>
-      </c>
-      <c r="R24" s="31"/>
-      <c r="S24" s="31"/>
-      <c r="T24" s="31"/>
-      <c r="U24" s="31"/>
-      <c r="V24" s="31"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="31"/>
-      <c r="Z24" s="31"/>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="31"/>
-      <c r="AC24" s="31"/>
-      <c r="AD24" s="31"/>
-      <c r="AE24" s="31"/>
-      <c r="AF24" s="31"/>
-      <c r="AG24" s="31"/>
-      <c r="AH24" s="31"/>
-      <c r="AI24" s="31"/>
-      <c r="AJ24" s="33"/>
-      <c r="AK24" s="4"/>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>61</v>
@@ -2501,53 +1314,8 @@
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="4"/>
-      <c r="J25" s="29">
-        <f>MEDIAN(L25:AJ25)</f>
-        <v>0.39312499999999995</v>
-      </c>
-      <c r="K25" t="s">
-        <v>78</v>
-      </c>
-      <c r="L25" s="29">
-        <v>2.2222222222222223E-2</v>
-      </c>
-      <c r="M25" s="30">
-        <v>0.25746527777777778</v>
-      </c>
-      <c r="N25" s="30">
-        <v>0.38452546296296292</v>
-      </c>
-      <c r="O25" s="30">
-        <v>0.40172453703703703</v>
-      </c>
-      <c r="P25" s="30">
-        <v>0.48754629629629626</v>
-      </c>
-      <c r="Q25" s="30">
-        <v>0.65498842592592588</v>
-      </c>
-      <c r="R25" s="31"/>
-      <c r="S25" s="31"/>
-      <c r="T25" s="31"/>
-      <c r="U25" s="31"/>
-      <c r="V25" s="31"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="31"/>
-      <c r="Y25" s="31"/>
-      <c r="Z25" s="31"/>
-      <c r="AA25" s="31"/>
-      <c r="AB25" s="31"/>
-      <c r="AC25" s="31"/>
-      <c r="AD25" s="31"/>
-      <c r="AE25" s="31"/>
-      <c r="AF25" s="31"/>
-      <c r="AG25" s="31"/>
-      <c r="AH25" s="31"/>
-      <c r="AI25" s="31"/>
-      <c r="AJ25" s="33"/>
-      <c r="AK25" s="4"/>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>62</v>
@@ -2565,53 +1333,8 @@
       </c>
       <c r="H26" s="16"/>
       <c r="I26" s="4"/>
-      <c r="J26" s="29">
-        <f>MEDIAN(L26:AJ26)</f>
-        <v>0.39505787037037038</v>
-      </c>
-      <c r="K26" t="s">
-        <v>87</v>
-      </c>
-      <c r="L26" s="29">
-        <v>3.7245370370370366E-2</v>
-      </c>
-      <c r="M26" s="30">
-        <v>0.22336805555555553</v>
-      </c>
-      <c r="N26" s="30">
-        <v>0.30394675925925924</v>
-      </c>
-      <c r="O26" s="30">
-        <v>0.48616898148148152</v>
-      </c>
-      <c r="P26" s="30">
-        <v>0.88638888888888889</v>
-      </c>
-      <c r="Q26" s="30">
-        <v>1.1883796296296296</v>
-      </c>
-      <c r="R26" s="31"/>
-      <c r="S26" s="31"/>
-      <c r="T26" s="31"/>
-      <c r="U26" s="31"/>
-      <c r="V26" s="31"/>
-      <c r="W26" s="31"/>
-      <c r="X26" s="31"/>
-      <c r="Y26" s="31"/>
-      <c r="Z26" s="31"/>
-      <c r="AA26" s="31"/>
-      <c r="AB26" s="31"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="31"/>
-      <c r="AE26" s="31"/>
-      <c r="AF26" s="31"/>
-      <c r="AG26" s="31"/>
-      <c r="AH26" s="31"/>
-      <c r="AI26" s="31"/>
-      <c r="AJ26" s="33"/>
-      <c r="AK26" s="4"/>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>63</v>
@@ -2629,35 +1352,8 @@
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="4"/>
-      <c r="J27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="31"/>
-      <c r="Q27" s="31"/>
-      <c r="R27" s="31"/>
-      <c r="S27" s="31"/>
-      <c r="T27" s="31"/>
-      <c r="U27" s="31"/>
-      <c r="V27" s="31"/>
-      <c r="W27" s="31"/>
-      <c r="X27" s="31"/>
-      <c r="Y27" s="31"/>
-      <c r="Z27" s="31"/>
-      <c r="AA27" s="31"/>
-      <c r="AB27" s="31"/>
-      <c r="AC27" s="31"/>
-      <c r="AD27" s="31"/>
-      <c r="AE27" s="31"/>
-      <c r="AF27" s="31"/>
-      <c r="AG27" s="31"/>
-      <c r="AH27" s="31"/>
-      <c r="AI27" s="31"/>
-      <c r="AJ27" s="33"/>
-      <c r="AK27" s="4"/>
-    </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>64</v>
@@ -2675,35 +1371,8 @@
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="31"/>
-      <c r="Q28" s="31"/>
-      <c r="R28" s="31"/>
-      <c r="S28" s="31"/>
-      <c r="T28" s="31"/>
-      <c r="U28" s="31"/>
-      <c r="V28" s="31"/>
-      <c r="W28" s="31"/>
-      <c r="X28" s="31"/>
-      <c r="Y28" s="31"/>
-      <c r="Z28" s="31"/>
-      <c r="AA28" s="31"/>
-      <c r="AB28" s="31"/>
-      <c r="AC28" s="31"/>
-      <c r="AD28" s="31"/>
-      <c r="AE28" s="31"/>
-      <c r="AF28" s="31"/>
-      <c r="AG28" s="31"/>
-      <c r="AH28" s="31"/>
-      <c r="AI28" s="31"/>
-      <c r="AJ28" s="33"/>
-      <c r="AK28" s="4"/>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>65</v>
@@ -2721,154 +1390,91 @@
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="4"/>
-      <c r="J29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
-      <c r="Q29" s="31"/>
-      <c r="R29" s="31"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="31"/>
-      <c r="U29" s="31"/>
-      <c r="V29" s="31"/>
-      <c r="W29" s="31"/>
-      <c r="X29" s="31"/>
-      <c r="Y29" s="31"/>
-      <c r="Z29" s="31"/>
-      <c r="AA29" s="31"/>
-      <c r="AB29" s="31"/>
-      <c r="AC29" s="31"/>
-      <c r="AD29" s="31"/>
-      <c r="AE29" s="31"/>
-      <c r="AF29" s="31"/>
-      <c r="AG29" s="31"/>
-      <c r="AH29" s="31"/>
-      <c r="AI29" s="31"/>
-      <c r="AJ29" s="33"/>
-      <c r="AK29" s="4"/>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="40"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="31"/>
-      <c r="N30" s="31"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="31"/>
-      <c r="Q30" s="31"/>
-      <c r="R30" s="31"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="31"/>
-      <c r="U30" s="31"/>
-      <c r="V30" s="31"/>
-      <c r="W30" s="31"/>
-      <c r="X30" s="31"/>
-      <c r="Y30" s="31"/>
-      <c r="Z30" s="31"/>
-      <c r="AA30" s="31"/>
-      <c r="AB30" s="31"/>
-      <c r="AC30" s="31"/>
-      <c r="AD30" s="31"/>
-      <c r="AE30" s="31"/>
-      <c r="AF30" s="31"/>
-      <c r="AG30" s="31"/>
-      <c r="AH30" s="31"/>
-      <c r="AI30" s="31"/>
-      <c r="AJ30" s="33"/>
-      <c r="AK30" s="4"/>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A31" s="41"/>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="AK31" s="4"/>
-    </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D32" s="24"/>
       <c r="E32" s="23"/>
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
       <c r="I32" s="4"/>
-      <c r="AK32" s="4"/>
-    </row>
-    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I33" s="4"/>
-      <c r="AK33" s="4"/>
-    </row>
-    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I34" s="4"/>
-      <c r="AK34" s="4"/>
-    </row>
-    <row r="35" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I35" s="4"/>
-      <c r="AK35" s="4"/>
-    </row>
-    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E36" s="25"/>
       <c r="I36" s="4"/>
-      <c r="AK36" s="4"/>
-    </row>
-    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E37" s="25"/>
       <c r="I37" s="4"/>
-      <c r="AK37" s="4"/>
-    </row>
-    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E38" s="25"/>
       <c r="I38" s="4"/>
-      <c r="AK38" s="4"/>
-    </row>
-    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E39" s="25"/>
       <c r="I39" s="4"/>
-      <c r="AK39" s="4"/>
-    </row>
-    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E40" s="25"/>
       <c r="I40" s="4"/>
     </row>
-    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E41" s="25"/>
       <c r="I41" s="4"/>
     </row>
-    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E42" s="25"/>
       <c r="I42" s="4"/>
     </row>
-    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E43" s="26"/>
       <c r="I43" s="4"/>
     </row>
-    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I44" s="4"/>
     </row>
-    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="25"/>
       <c r="I45" s="4"/>
     </row>
-    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I46" s="4"/>
     </row>
-    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I47" s="4"/>
     </row>
-    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I48" s="4"/>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.25">
@@ -2884,9 +1490,6 @@
       <c r="I52" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="J5:Q26">
-    <sortCondition ref="J5:J26"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated viz for Day 7.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 7: TITLE</t>
-  </si>
-  <si>
     <t>Day 8: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 6: Universal Orbit Map</t>
+  </si>
+  <si>
+    <t>Day 7: Amplification Circuit</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,26 +1033,34 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C11" s="2">
+        <v>8.0555555555555554E-3</v>
+      </c>
       <c r="D11" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="22"/>
+        <v>3.3148148148148149E-2</v>
+      </c>
+      <c r="E11" s="16">
+        <v>4.1203703703703708E-2</v>
+      </c>
+      <c r="F11" s="22">
+        <v>2.1435185185185186E-2</v>
+      </c>
       <c r="G11" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="16"/>
+        <v>1.9768518518518522E-2</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1071,7 +1079,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1090,7 +1098,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1109,7 +1117,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1128,7 +1136,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1147,7 +1155,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1166,7 +1174,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1185,7 +1193,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1204,7 +1212,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1223,7 +1231,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1242,7 +1250,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1261,7 +1269,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1280,7 +1288,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1299,7 +1307,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1318,7 +1326,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1337,7 +1345,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1356,7 +1364,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1375,7 +1383,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz to obfuscate names in source code of published webpage.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 8: TITLE</t>
-  </si>
-  <si>
     <t>Day 9: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 7: Amplification Circuit</t>
+  </si>
+  <si>
+    <t>Day 8: Space Image Format</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,26 +1060,34 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C12" s="2">
+        <v>7.3726851851851861E-3</v>
+      </c>
       <c r="D12" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="22"/>
+        <v>1.4004629629629631E-2</v>
+      </c>
+      <c r="E12" s="16">
+        <v>2.1377314814814818E-2</v>
+      </c>
+      <c r="F12" s="22">
+        <v>6.4004629629629628E-3</v>
+      </c>
       <c r="G12" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="16"/>
+        <v>1.4976851851851856E-2</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1098,7 +1106,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1117,7 +1125,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1136,7 +1144,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1155,7 +1163,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1174,7 +1182,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1193,7 +1201,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1212,7 +1220,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1231,7 +1239,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1250,7 +1258,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1269,7 +1277,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1288,7 +1296,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1307,7 +1315,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1326,7 +1334,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1345,7 +1353,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1364,7 +1372,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1383,7 +1391,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 10.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 9: TITLE</t>
-  </si>
-  <si>
     <t>Day 10: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 8: Space Image Format</t>
+  </si>
+  <si>
+    <t>Day 9: Sensor Boost</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,26 +1087,34 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.8692129629629631E-2</v>
+      </c>
       <c r="D13" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="22"/>
+        <v>1.1342592592592585E-3</v>
+      </c>
+      <c r="E13" s="16">
+        <v>1.982638888888889E-2</v>
+      </c>
+      <c r="F13" s="22">
+        <v>1.6851851851851851E-2</v>
+      </c>
       <c r="G13" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="16"/>
+        <v>2.9745370370370394E-3</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1125,7 +1133,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1144,7 +1152,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1163,7 +1171,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1182,7 +1190,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1201,7 +1209,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1220,7 +1228,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1239,7 +1247,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1258,7 +1266,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1277,7 +1285,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1296,7 +1304,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1315,7 +1323,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1334,7 +1342,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1353,7 +1361,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1372,7 +1380,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1391,7 +1399,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Added link to global leaderboard for global times.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 10: TITLE</t>
-  </si>
-  <si>
     <t>Day 11: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 9: Sensor Boost</t>
+  </si>
+  <si>
+    <t>Day 10: Monitoring Station</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,26 +1114,34 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4.5069444444444447E-2</v>
+      </c>
       <c r="D14" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="22"/>
+        <v>2.0706018518518519E-2</v>
+      </c>
+      <c r="E14" s="16">
+        <v>6.5775462962962966E-2</v>
+      </c>
+      <c r="F14" s="22">
+        <v>1.8124999999999999E-2</v>
+      </c>
       <c r="G14" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="16"/>
+        <v>4.7650462962962964E-2</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1152,7 +1160,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1171,7 +1179,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1190,7 +1198,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1209,7 +1217,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1228,7 +1236,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1247,7 +1255,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1266,7 +1274,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1285,7 +1293,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1304,7 +1312,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1323,7 +1331,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1342,7 +1350,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1361,7 +1369,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1380,7 +1388,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1399,7 +1407,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz to show first, second, and third place finishes with median times.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 11: TITLE</t>
-  </si>
-  <si>
     <t>Day 12: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 10: Monitoring Station</t>
+  </si>
+  <si>
+    <t>Day 11: Space Police</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,26 +1141,34 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.6446759259259262E-2</v>
+      </c>
       <c r="D15" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="22"/>
+        <v>2.5925925925925908E-3</v>
+      </c>
+      <c r="E15" s="16">
+        <v>1.9039351851851852E-2</v>
+      </c>
+      <c r="F15" s="22">
+        <v>9.9537037037037042E-3</v>
+      </c>
       <c r="G15" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="16"/>
+        <v>9.0856481481481483E-3</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1179,7 +1187,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1198,7 +1206,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1217,7 +1225,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1236,7 +1244,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1255,7 +1263,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1274,7 +1282,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1293,7 +1301,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1312,7 +1320,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1331,7 +1339,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1350,7 +1358,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1369,7 +1377,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1388,7 +1396,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1407,7 +1415,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 12.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 12: TITLE</t>
-  </si>
-  <si>
     <t>Day 13: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 11: Space Police</t>
+  </si>
+  <si>
+    <t>Day 12: The N-Body Problem</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,26 +1168,34 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1.1469907407407408E-2</v>
+      </c>
       <c r="D16" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="16"/>
-      <c r="F16" s="22"/>
+        <v>2.6851851851851849E-2</v>
+      </c>
+      <c r="E16" s="16">
+        <v>3.8321759259259257E-2</v>
+      </c>
+      <c r="F16" s="22">
+        <v>2.461805555555556E-2</v>
+      </c>
       <c r="G16" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="16"/>
+        <v>1.3703703703703697E-2</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1206,7 +1214,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1225,7 +1233,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1244,7 +1252,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1263,7 +1271,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1282,7 +1290,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1301,7 +1309,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1320,7 +1328,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1339,7 +1347,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1358,7 +1366,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1377,7 +1385,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1396,7 +1404,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1415,7 +1423,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 13.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 13: TITLE</t>
-  </si>
-  <si>
     <t>Day 14: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 12: The N-Body Problem</t>
+  </si>
+  <si>
+    <t>Day 13: Care Package</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,13 +1060,13 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
       </c>
       <c r="D12" s="15">
-        <f t="shared" si="0"/>
+        <f>E12-C12</f>
         <v>1.4004629629629631E-2</v>
       </c>
       <c r="E12" s="16">
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,26 +1195,34 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C17" s="2">
+        <v>5.0810185185185186E-3</v>
+      </c>
       <c r="D17" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="22"/>
+        <v>3.4756944444444444E-2</v>
+      </c>
+      <c r="E17" s="16">
+        <v>3.9837962962962964E-2</v>
+      </c>
+      <c r="F17" s="22">
+        <v>1.9861111111111111E-2</v>
+      </c>
       <c r="G17" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="16"/>
+        <v>1.9976851851851853E-2</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1233,7 +1241,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1252,7 +1260,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1271,7 +1279,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1290,7 +1298,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1309,7 +1317,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1328,7 +1336,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1347,7 +1355,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1366,7 +1374,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1385,7 +1393,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1404,7 +1412,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1423,7 +1431,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 14.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 14: TITLE</t>
-  </si>
-  <si>
     <t>Day 15: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 13: Care Package</t>
+  </si>
+  <si>
+    <t>Day 14: Space Stoichiometry</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,26 +1222,34 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6.1504629629629631E-2</v>
+      </c>
       <c r="D18" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="22"/>
+        <v>2.7002314814814812E-2</v>
+      </c>
+      <c r="E18" s="16">
+        <v>8.8506944444444444E-2</v>
+      </c>
+      <c r="F18" s="22">
+        <v>4.8773148148148149E-2</v>
+      </c>
       <c r="G18" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="16"/>
+        <v>3.9733796296296295E-2</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1260,7 +1268,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1279,7 +1287,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1298,7 +1306,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1317,7 +1325,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1336,7 +1344,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1355,7 +1363,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1374,7 +1382,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1393,7 +1401,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1412,7 +1420,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1431,7 +1439,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz to show all puzzle times for top players.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 15: TITLE</t>
-  </si>
-  <si>
     <t>Day 16: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 14: Space Stoichiometry</t>
+  </si>
+  <si>
+    <t>Day 15: Oxygen System</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,26 +1249,34 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C19" s="2">
+        <v>8.3194444444444446E-2</v>
+      </c>
       <c r="D19" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="22"/>
+        <v>2.5706018518518517E-2</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0.10890046296296296</v>
+      </c>
+      <c r="F19" s="22">
+        <v>4.5590277777777778E-2</v>
+      </c>
       <c r="G19" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="16"/>
+        <v>6.3310185185185192E-2</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1287,7 +1295,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1306,7 +1314,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1325,7 +1333,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1344,7 +1352,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1363,7 +1371,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1382,7 +1390,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1401,7 +1409,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1420,7 +1428,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1439,7 +1447,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 16.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 16: TITLE</t>
-  </si>
-  <si>
     <t>Day 17: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 15: Oxygen System</t>
+  </si>
+  <si>
+    <t>Day 16: Flawed Frequency Transmission</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,26 +1276,34 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C20" s="2">
+        <v>2.8854166666666667E-2</v>
+      </c>
       <c r="D20" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="22"/>
+        <v>6.1030092592592594E-2</v>
+      </c>
+      <c r="E20" s="16">
+        <v>8.9884259259259261E-2</v>
+      </c>
+      <c r="F20" s="22">
+        <v>7.7199074074074073E-2</v>
+      </c>
       <c r="G20" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="16"/>
+        <v>1.2685185185185188E-2</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1314,7 +1322,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1333,7 +1341,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1352,7 +1360,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1371,7 +1379,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1390,7 +1398,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1409,7 +1417,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1428,7 +1436,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1447,7 +1455,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 17.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 17: TITLE</t>
-  </si>
-  <si>
     <t>Day 18: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 16: Flawed Frequency Transmission</t>
+  </si>
+  <si>
+    <t>Day 17: Set and Forget</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,26 +1303,34 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1.1898148148148149E-2</v>
+      </c>
       <c r="D21" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="22"/>
+        <v>2.7094907407407401E-2</v>
+      </c>
+      <c r="E21" s="16">
+        <v>3.8993055555555552E-2</v>
+      </c>
+      <c r="F21" s="22">
+        <v>3.5277777777777776E-2</v>
+      </c>
       <c r="G21" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="16"/>
+        <v>3.7152777777777757E-3</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1341,7 +1349,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1360,7 +1368,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1379,7 +1387,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1398,7 +1406,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1417,7 +1425,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1436,7 +1444,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1455,7 +1463,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 18.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 18: TITLE</t>
-  </si>
-  <si>
     <t>Day 19: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 17: Set and Forget</t>
+  </si>
+  <si>
+    <t>Day 18: Many-Worlds Interpretation</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,26 +1330,34 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.12148148148148148</v>
+      </c>
       <c r="D22" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="22"/>
+        <v>7.1504629629629626E-2</v>
+      </c>
+      <c r="E22" s="16">
+        <v>0.19298611111111111</v>
+      </c>
+      <c r="F22" s="22">
+        <v>0.1706134259259259</v>
+      </c>
       <c r="G22" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="16"/>
+        <v>2.2372685185185204E-2</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1368,7 +1376,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1387,7 +1395,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1406,7 +1414,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1425,7 +1433,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1444,7 +1452,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1463,7 +1471,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 19.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 19: TITLE</t>
-  </si>
-  <si>
     <t>Day 20: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 18: Many-Worlds Interpretation</t>
+  </si>
+  <si>
+    <t>Day 19: Tractor Beam</t>
   </si>
 </sst>
 </file>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,7 +1330,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2">
         <v>0.12148148148148148</v>
@@ -1357,26 +1357,34 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6.238425925925925E-3</v>
+      </c>
       <c r="D23" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="22"/>
+        <v>2.7118055555555555E-2</v>
+      </c>
+      <c r="E23" s="16">
+        <v>3.335648148148148E-2</v>
+      </c>
+      <c r="F23" s="22">
+        <v>3.006944444444444E-2</v>
+      </c>
       <c r="G23" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="16"/>
+        <v>3.2870370370370397E-3</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1395,7 +1403,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1414,7 +1422,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1433,7 +1441,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1452,7 +1460,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1471,7 +1479,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 20.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 20: TITLE</t>
-  </si>
-  <si>
     <t>Day 21: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 19: Tractor Beam</t>
+  </si>
+  <si>
+    <t>Day 20: Donut Maze</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,7 +1330,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C22" s="2">
         <v>0.12148148148148148</v>
@@ -1357,7 +1357,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="2">
         <v>6.238425925925925E-3</v>
@@ -1384,26 +1384,34 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2.7696759259259258E-2</v>
+      </c>
       <c r="D24" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="22"/>
+        <v>2.8935185185185185E-2</v>
+      </c>
+      <c r="E24" s="16">
+        <v>5.6631944444444443E-2</v>
+      </c>
+      <c r="F24" s="22">
+        <v>4.3356481481481475E-2</v>
+      </c>
       <c r="G24" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="16"/>
+        <v>1.3275462962962968E-2</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1422,7 +1430,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1441,7 +1449,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1460,7 +1468,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1479,7 +1487,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 21.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 21: TITLE</t>
-  </si>
-  <si>
     <t>Day 22: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 20: Donut Maze</t>
+  </si>
+  <si>
+    <t>Day 21: Springdroid Adventure</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,7 +1330,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="2">
         <v>0.12148148148148148</v>
@@ -1357,7 +1357,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="2">
         <v>6.238425925925925E-3</v>
@@ -1384,7 +1384,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="2">
         <v>2.7696759259259258E-2</v>
@@ -1411,7 +1411,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1419,10 +1419,12 @@
         <v>0</v>
       </c>
       <c r="E25" s="16"/>
-      <c r="F25" s="22"/>
+      <c r="F25" s="22">
+        <v>1.9814814814814816E-2</v>
+      </c>
       <c r="G25" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1.9814814814814816E-2</v>
       </c>
       <c r="H25" s="16"/>
       <c r="I25" s="4"/>
@@ -1430,7 +1432,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1449,7 +1451,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1468,7 +1470,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1487,7 +1489,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for day 22.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 22: TITLE</t>
-  </si>
-  <si>
     <t>Day 23: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 21: Springdroid Adventure</t>
+  </si>
+  <si>
+    <t>Day 22: Slam Shuffle</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,7 +1330,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2">
         <v>0.12148148148148148</v>
@@ -1357,7 +1357,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C23" s="2">
         <v>6.238425925925925E-3</v>
@@ -1384,7 +1384,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C24" s="2">
         <v>2.7696759259259258E-2</v>
@@ -1411,47 +1411,61 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2.6770833333333331E-2</v>
+      </c>
       <c r="D25" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="16"/>
+        <v>9.9537037037037042E-3</v>
+      </c>
+      <c r="E25" s="16">
+        <v>3.6724537037037035E-2</v>
+      </c>
       <c r="F25" s="22">
         <v>1.9814814814814816E-2</v>
       </c>
       <c r="G25" s="22">
         <f t="shared" si="1"/>
-        <v>-1.9814814814814816E-2</v>
-      </c>
-      <c r="H25" s="16"/>
+        <v>1.6909722222222218E-2</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.2685185185185183E-2</v>
+      </c>
       <c r="D26" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="22"/>
+        <v>0.12690972222222224</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0.14959490740740741</v>
+      </c>
+      <c r="F26" s="22">
+        <v>0.1292939814814815</v>
+      </c>
       <c r="G26" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="16"/>
+        <v>2.0300925925925917E-2</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1470,7 +1484,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1489,7 +1503,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 23.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 23: TITLE</t>
-  </si>
-  <si>
     <t>Day 24: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 22: Slam Shuffle</t>
+  </si>
+  <si>
+    <t>Day 23: Category Six</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,7 +1330,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="2">
         <v>0.12148148148148148</v>
@@ -1357,7 +1357,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C23" s="2">
         <v>6.238425925925925E-3</v>
@@ -1384,7 +1384,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2">
         <v>2.7696759259259258E-2</v>
@@ -1411,7 +1411,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="2">
         <v>2.6770833333333331E-2</v>
@@ -1438,7 +1438,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="2">
         <v>2.2685185185185183E-2</v>
@@ -1465,26 +1465,34 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2.9062500000000002E-2</v>
+      </c>
       <c r="D27" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="22"/>
+        <v>9.0972222222222253E-3</v>
+      </c>
+      <c r="E27" s="16">
+        <v>3.8159722222222227E-2</v>
+      </c>
+      <c r="F27" s="22">
+        <v>2.2534722222222223E-2</v>
+      </c>
       <c r="G27" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="16"/>
+        <v>1.5625000000000003E-2</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1503,7 +1511,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 24.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 24: TITLE</t>
-  </si>
-  <si>
     <t>Day 25: TITLE</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 23: Category Six</t>
+  </si>
+  <si>
+    <t>Day 24: Planet of Discord</t>
   </si>
 </sst>
 </file>
@@ -789,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,7 +1330,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="2">
         <v>0.12148148148148148</v>
@@ -1357,7 +1357,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2">
         <v>6.238425925925925E-3</v>
@@ -1384,7 +1384,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2">
         <v>2.7696759259259258E-2</v>
@@ -1411,7 +1411,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="2">
         <v>2.6770833333333331E-2</v>
@@ -1438,7 +1438,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="2">
         <v>2.2685185185185183E-2</v>
@@ -1465,7 +1465,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="2">
         <v>2.9062500000000002E-2</v>
@@ -1492,26 +1492,34 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.4756944444444446E-2</v>
+      </c>
       <c r="D28" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="22"/>
+        <v>4.1423611111111112E-2</v>
+      </c>
+      <c r="E28" s="16">
+        <v>5.618055555555556E-2</v>
+      </c>
+      <c r="F28" s="22">
+        <v>2.4641203703703703E-2</v>
+      </c>
       <c r="G28" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="16"/>
+        <v>3.153935185185186E-2</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz for Day 25.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
   <si>
     <t>Puzzle</t>
   </si>
@@ -158,9 +158,6 @@
     <t>Finish</t>
   </si>
   <si>
-    <t>Day 25: TITLE</t>
-  </si>
-  <si>
     <t>Day 1: The Tyranny of the Rocket Equation</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Day 24: Planet of Discord</t>
+  </si>
+  <si>
+    <t>Day 25: Cryostasis</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +871,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2">
         <v>1.6435185185185183E-3</v>
@@ -898,7 +898,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="2">
         <v>6.782407407407408E-3</v>
@@ -925,7 +925,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="2">
         <v>1.5381944444444443E-2</v>
@@ -952,7 +952,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2">
         <v>3.37962962962963E-3</v>
@@ -972,14 +972,14 @@
         <v>1.7407407407407413E-2</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2">
         <v>1.9201388888888889E-2</v>
@@ -1006,7 +1006,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2">
         <v>6.7245370370370367E-3</v>
@@ -1033,7 +1033,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2">
         <v>8.0555555555555554E-3</v>
@@ -1060,7 +1060,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2">
         <v>7.3726851851851861E-3</v>
@@ -1087,7 +1087,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2">
         <v>1.8692129629629631E-2</v>
@@ -1114,7 +1114,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2">
         <v>4.5069444444444447E-2</v>
@@ -1141,7 +1141,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2">
         <v>1.6446759259259262E-2</v>
@@ -1168,7 +1168,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2">
         <v>1.1469907407407408E-2</v>
@@ -1195,7 +1195,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="2">
         <v>5.0810185185185186E-3</v>
@@ -1222,7 +1222,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2">
         <v>6.1504629629629631E-2</v>
@@ -1249,7 +1249,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2">
         <v>8.3194444444444446E-2</v>
@@ -1276,7 +1276,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C20" s="2">
         <v>2.8854166666666667E-2</v>
@@ -1303,7 +1303,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="2">
         <v>1.1898148148148149E-2</v>
@@ -1330,7 +1330,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="2">
         <v>0.12148148148148148</v>
@@ -1357,7 +1357,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="2">
         <v>6.238425925925925E-3</v>
@@ -1384,7 +1384,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="2">
         <v>2.7696759259259258E-2</v>
@@ -1411,7 +1411,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C25" s="2">
         <v>2.6770833333333331E-2</v>
@@ -1438,7 +1438,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" s="2">
         <v>2.2685185185185183E-2</v>
@@ -1465,7 +1465,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" s="2">
         <v>2.9062500000000002E-2</v>
@@ -1492,7 +1492,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2">
         <v>1.4756944444444446E-2</v>
@@ -1519,20 +1519,28 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2.2372685185185186E-2</v>
+      </c>
       <c r="D29" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="22"/>
+        <v>4.6296296296294281E-5</v>
+      </c>
+      <c r="E29" s="16">
+        <v>2.2418981481481481E-2</v>
+      </c>
+      <c r="F29" s="22">
+        <v>1.050925925925926E-2</v>
+      </c>
       <c r="G29" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H29" s="16"/>
+        <v>1.1909722222222221E-2</v>
+      </c>
+      <c r="H29" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set up for y20.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="12435" windowHeight="4695"/>
   </bookViews>
   <sheets>
-    <sheet name="2019" sheetId="2" r:id="rId1"/>
-    <sheet name="2018" sheetId="1" r:id="rId2"/>
+    <sheet name="2020" sheetId="3" r:id="rId1"/>
+    <sheet name="2019" sheetId="2" r:id="rId2"/>
+    <sheet name="2018" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="98">
   <si>
     <t>Puzzle</t>
   </si>
@@ -234,6 +235,81 @@
   </si>
   <si>
     <t>Day 25: Cryostasis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 1: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 2: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 3: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 4: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 5: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 6: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 7: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 8: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 9: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 10: </t>
+  </si>
+  <si>
+    <t>Day 11:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 12: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 13: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 14: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 15: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 16: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 17: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 18: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 19: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 20: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 21: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 22: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 23: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 24: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day 25: </t>
   </si>
 </sst>
 </file>
@@ -789,7 +865,594 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" customWidth="1"/>
+    <col min="3" max="8" width="9.7109375" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" customWidth="1"/>
+    <col min="10" max="18" width="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="27"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21">
+        <f t="shared" ref="G5:G29" si="0">E5-F5</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="28"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="28"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="16"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="16"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="16"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="16"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="16"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="16"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="16"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="16"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="16"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="16"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="16"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="16"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H21" s="16"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="16"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="16"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H28" s="16"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="16"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D32" s="24"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="I32" s="4"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="4"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="4"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E36" s="25"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E37" s="25"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E38" s="25"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E39" s="25"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E40" s="25"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E41" s="25"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E42" s="25"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E43" s="26"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="25"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
@@ -1647,7 +2310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I46"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated viz for y20d01.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 1: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 2: </t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t xml:space="preserve">Day 25: </t>
+  </si>
+  <si>
+    <t>Day 1: Report Repair</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,30 +947,41 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="21"/>
+        <v>97</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.29097222222222224</v>
+      </c>
+      <c r="D5" s="15">
+        <f t="shared" ref="D5" si="0">E5-C5</f>
+        <v>2.777777777777779E-2</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.31875000000000003</v>
+      </c>
+      <c r="F5" s="21">
+        <v>0.31875000000000003</v>
+      </c>
       <c r="G5" s="21">
-        <f t="shared" ref="G5:G29" si="0">E5-F5</f>
+        <f t="shared" ref="G5:G29" si="1">E5-F5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="28"/>
+      <c r="H5" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="21"/>
       <c r="G6" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H6" s="28"/>
@@ -979,14 +990,14 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
       <c r="F7" s="22"/>
       <c r="G7" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H7" s="16"/>
@@ -995,14 +1006,14 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
       <c r="F8" s="22"/>
       <c r="G8" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H8" s="16"/>
@@ -1011,14 +1022,14 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H9" s="16"/>
@@ -1027,14 +1038,14 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H10" s="16"/>
@@ -1043,14 +1054,14 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H11" s="16"/>
@@ -1059,14 +1070,14 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H12" s="16"/>
@@ -1075,14 +1086,14 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H13" s="16"/>
@@ -1091,14 +1102,14 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H14" s="16"/>
@@ -1107,14 +1118,14 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H15" s="16"/>
@@ -1123,14 +1134,14 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H16" s="16"/>
@@ -1139,14 +1150,14 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H17" s="16"/>
@@ -1155,14 +1166,14 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15"/>
       <c r="E18" s="16"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H18" s="16"/>
@@ -1171,14 +1182,14 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H19" s="16"/>
@@ -1187,14 +1198,14 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H20" s="16"/>
@@ -1203,14 +1214,14 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H21" s="16"/>
@@ -1219,14 +1230,14 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15"/>
       <c r="E22" s="16"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H22" s="16"/>
@@ -1235,14 +1246,14 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H23" s="16"/>
@@ -1251,14 +1262,14 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15"/>
       <c r="E24" s="16"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H24" s="16"/>
@@ -1267,14 +1278,14 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H25" s="16"/>
@@ -1283,14 +1294,14 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H26" s="16"/>
@@ -1299,14 +1310,14 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H27" s="16"/>
@@ -1315,14 +1326,14 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H28" s="16"/>
@@ -1331,14 +1342,14 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15"/>
       <c r="E29" s="16"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H29" s="16"/>
@@ -1452,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated viz with y20d02 results and new links.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 2: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 3: </t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t>Day 1: Report Repair</t>
+  </si>
+  <si>
+    <t>Day 2: Password Philosophy</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,13 +947,13 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2">
         <v>0.29097222222222224</v>
       </c>
       <c r="D5" s="15">
-        <f t="shared" ref="D5" si="0">E5-C5</f>
+        <f t="shared" ref="D5:D29" si="0">E5-C5</f>
         <v>2.777777777777779E-2</v>
       </c>
       <c r="E5" s="16">
@@ -974,26 +974,40 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="21"/>
+        <v>97</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.17916666666666667</v>
+      </c>
+      <c r="D6" s="15">
+        <f t="shared" si="0"/>
+        <v>0.11319444444444446</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.29236111111111113</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0.25694444444444448</v>
+      </c>
       <c r="G6" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="28"/>
+        <v>3.5416666666666652E-2</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>7</v>
+      </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="15"/>
+      <c r="D7" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E7" s="16"/>
       <c r="F7" s="22"/>
       <c r="G7" s="21">
@@ -1006,10 +1020,13 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E8" s="16"/>
       <c r="F8" s="22"/>
       <c r="G8" s="21">
@@ -1022,10 +1039,13 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="15"/>
+      <c r="D9" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E9" s="16"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22">
@@ -1038,10 +1058,13 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="15"/>
+      <c r="D10" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E10" s="16"/>
       <c r="F10" s="22"/>
       <c r="G10" s="22">
@@ -1054,10 +1077,13 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E11" s="16"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22">
@@ -1070,10 +1096,13 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E12" s="16"/>
       <c r="F12" s="22"/>
       <c r="G12" s="22">
@@ -1086,10 +1115,13 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E13" s="16"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22">
@@ -1102,10 +1134,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E14" s="16"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22">
@@ -1118,10 +1153,13 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E15" s="16"/>
       <c r="F15" s="22"/>
       <c r="G15" s="22">
@@ -1134,10 +1172,13 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E16" s="16"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22">
@@ -1150,10 +1191,13 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E17" s="16"/>
       <c r="F17" s="22"/>
       <c r="G17" s="22">
@@ -1166,10 +1210,13 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="15"/>
+      <c r="D18" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E18" s="16"/>
       <c r="F18" s="22"/>
       <c r="G18" s="22">
@@ -1182,10 +1229,13 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="15"/>
+      <c r="D19" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E19" s="16"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22">
@@ -1198,10 +1248,13 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="15"/>
+      <c r="D20" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E20" s="16"/>
       <c r="F20" s="22"/>
       <c r="G20" s="22">
@@ -1214,10 +1267,13 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="15"/>
+      <c r="D21" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E21" s="16"/>
       <c r="F21" s="22"/>
       <c r="G21" s="22">
@@ -1230,10 +1286,13 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="15"/>
+      <c r="D22" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E22" s="16"/>
       <c r="F22" s="22"/>
       <c r="G22" s="22">
@@ -1246,10 +1305,13 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="15"/>
+      <c r="D23" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E23" s="16"/>
       <c r="F23" s="22"/>
       <c r="G23" s="22">
@@ -1262,10 +1324,13 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="15"/>
+      <c r="D24" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E24" s="16"/>
       <c r="F24" s="22"/>
       <c r="G24" s="22">
@@ -1278,10 +1343,13 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="15"/>
+      <c r="D25" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E25" s="16"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22">
@@ -1294,10 +1362,13 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="15"/>
+      <c r="D26" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E26" s="16"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22">
@@ -1310,10 +1381,13 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2"/>
-      <c r="D27" s="15"/>
+      <c r="D27" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E27" s="16"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22">
@@ -1326,10 +1400,13 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="2"/>
-      <c r="D28" s="15"/>
+      <c r="D28" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E28" s="16"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22">
@@ -1342,10 +1419,13 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" s="2"/>
-      <c r="D29" s="15"/>
+      <c r="D29" s="15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E29" s="16"/>
       <c r="F29" s="22"/>
       <c r="G29" s="22">

</xml_diff>

<commit_message>
Updated viz with y20d4 results.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,12 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 3: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day 4: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 5: </t>
   </si>
   <si>
@@ -310,6 +304,12 @@
   </si>
   <si>
     <t>Day 2: Password Philosophy</t>
+  </si>
+  <si>
+    <t>Day 3: Toboggan Trajectory</t>
+  </si>
+  <si>
+    <t>Day 4: Passport Processing</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +947,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2">
         <v>0.29097222222222224</v>
@@ -974,7 +974,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" s="2">
         <v>0.17916666666666667</v>
@@ -1001,45 +1001,61 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.3833333333333333</v>
+      </c>
       <c r="D7" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="22"/>
+        <v>0.14027777777777783</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.52361111111111114</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.26319444444444445</v>
+      </c>
       <c r="G7" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="16"/>
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>8</v>
+      </c>
       <c r="I7" s="4"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.54861111111111105</v>
+      </c>
       <c r="D8" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="16"/>
-      <c r="F8" s="22"/>
+        <v>0.75555555555555565</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1.3041666666666667</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.76666666666666661</v>
+      </c>
       <c r="G8" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="16"/>
+        <v>0.53750000000000009</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>15</v>
+      </c>
       <c r="I8" s="4"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="15">
@@ -1058,7 +1074,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15">
@@ -1077,7 +1093,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1096,7 +1112,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1115,7 +1131,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1134,7 +1150,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1153,7 +1169,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1172,7 +1188,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1191,7 +1207,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1210,7 +1226,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1229,7 +1245,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1248,7 +1264,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1267,7 +1283,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1286,7 +1302,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1305,7 +1321,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1324,7 +1340,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1343,7 +1359,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1362,7 +1378,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1381,7 +1397,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1400,7 +1416,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1419,7 +1435,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz with y20d05 results.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 5: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 6: </t>
   </si>
   <si>
@@ -310,6 +307,9 @@
   </si>
   <si>
     <t>Day 4: Passport Processing</t>
+  </si>
+  <si>
+    <t>Day 5: Binary Boarding</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +947,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2">
         <v>0.29097222222222224</v>
@@ -974,7 +974,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2">
         <v>0.17916666666666667</v>
@@ -1001,7 +1001,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2">
         <v>0.3833333333333333</v>
@@ -1028,7 +1028,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="2">
         <v>0.54861111111111105</v>
@@ -1055,26 +1055,34 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.57500000000000007</v>
+      </c>
       <c r="D9" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="22"/>
+        <v>0.14097222222222217</v>
+      </c>
+      <c r="E9" s="16">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="F9" s="22">
+        <v>0.42430555555555555</v>
+      </c>
       <c r="G9" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="15">
@@ -1093,7 +1101,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1112,7 +1120,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1131,7 +1139,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1150,7 +1158,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1169,7 +1177,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1188,7 +1196,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1207,7 +1215,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1226,7 +1234,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1245,7 +1253,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1264,7 +1272,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1283,7 +1291,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1302,7 +1310,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1321,7 +1329,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1340,7 +1348,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1359,7 +1367,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1378,7 +1386,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1397,7 +1405,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1416,7 +1424,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1435,7 +1443,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Added Day 6 to viz.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="99">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 6: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 7: </t>
   </si>
   <si>
@@ -310,6 +307,12 @@
   </si>
   <si>
     <t>Day 5: Binary Boarding</t>
+  </si>
+  <si>
+    <t>Day 6: Custom Customs</t>
+  </si>
+  <si>
+    <t>13th</t>
   </si>
 </sst>
 </file>
@@ -866,7 +869,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +950,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="2">
         <v>0.29097222222222224</v>
@@ -974,7 +977,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="2">
         <v>0.17916666666666667</v>
@@ -1001,7 +1004,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" s="2">
         <v>0.3833333333333333</v>
@@ -1028,7 +1031,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" s="2">
         <v>0.54861111111111105</v>
@@ -1055,7 +1058,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" s="2">
         <v>0.57500000000000007</v>
@@ -1082,26 +1085,34 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.53194444444444444</v>
+      </c>
       <c r="D10" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="22"/>
+        <v>7.7083333333333393E-2</v>
+      </c>
+      <c r="E10" s="16">
+        <v>0.60902777777777783</v>
+      </c>
+      <c r="F10" s="22">
+        <v>0.25555555555555559</v>
+      </c>
       <c r="G10" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H10" s="16"/>
+        <v>0.35347222222222224</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>98</v>
+      </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="15">
@@ -1120,7 +1131,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1139,7 +1150,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1158,7 +1169,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1177,7 +1188,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1196,7 +1207,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1215,7 +1226,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1234,7 +1245,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1253,7 +1264,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1272,7 +1283,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1291,7 +1302,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1310,7 +1321,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1329,7 +1340,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1348,7 +1359,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1367,7 +1378,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1386,7 +1397,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1405,7 +1416,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1424,7 +1435,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1443,7 +1454,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Added day 7 to viz.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="99">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 7: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 8: </t>
   </si>
   <si>
@@ -313,6 +310,9 @@
   </si>
   <si>
     <t>13th</t>
+  </si>
+  <si>
+    <t>Day 7: Handy Haversacks</t>
   </si>
 </sst>
 </file>
@@ -869,7 +869,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,20 +950,20 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2">
-        <v>0.29097222222222224</v>
+        <v>4.8495370370370368E-3</v>
       </c>
       <c r="D5" s="15">
         <f t="shared" ref="D5:D29" si="0">E5-C5</f>
-        <v>2.777777777777779E-2</v>
+        <v>4.6296296296296363E-4</v>
       </c>
       <c r="E5" s="16">
-        <v>0.31875000000000003</v>
+        <v>5.3125000000000004E-3</v>
       </c>
       <c r="F5" s="21">
-        <v>0.31875000000000003</v>
+        <v>5.3125000000000004E-3</v>
       </c>
       <c r="G5" s="21">
         <f t="shared" ref="G5:G29" si="1">E5-F5</f>
@@ -977,24 +977,24 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" s="2">
-        <v>0.17916666666666667</v>
+        <v>2.9861111111111113E-3</v>
       </c>
       <c r="D6" s="15">
         <f t="shared" si="0"/>
-        <v>0.11319444444444446</v>
+        <v>1.8865740740740744E-3</v>
       </c>
       <c r="E6" s="16">
-        <v>0.29236111111111113</v>
+        <v>4.8726851851851856E-3</v>
       </c>
       <c r="F6" s="21">
-        <v>0.25694444444444448</v>
+        <v>4.2824074074074075E-3</v>
       </c>
       <c r="G6" s="21">
         <f t="shared" si="1"/>
-        <v>3.5416666666666652E-2</v>
+        <v>5.9027777777777811E-4</v>
       </c>
       <c r="H6" s="28" t="s">
         <v>7</v>
@@ -1004,24 +1004,24 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="2">
-        <v>0.3833333333333333</v>
+        <v>6.3888888888888884E-3</v>
       </c>
       <c r="D7" s="15">
         <f t="shared" si="0"/>
-        <v>0.14027777777777783</v>
+        <v>2.3379629629629636E-3</v>
       </c>
       <c r="E7" s="16">
-        <v>0.52361111111111114</v>
+        <v>8.726851851851852E-3</v>
       </c>
       <c r="F7" s="22">
-        <v>0.26319444444444445</v>
+        <v>4.386574074074074E-3</v>
       </c>
       <c r="G7" s="21">
         <f t="shared" si="1"/>
-        <v>0.26041666666666669</v>
+        <v>4.340277777777778E-3</v>
       </c>
       <c r="H7" s="16" t="s">
         <v>8</v>
@@ -1031,24 +1031,24 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2">
-        <v>0.54861111111111105</v>
+        <v>9.1435185185185178E-3</v>
       </c>
       <c r="D8" s="15">
         <f t="shared" si="0"/>
-        <v>0.75555555555555565</v>
+        <v>1.2592592592592594E-2</v>
       </c>
       <c r="E8" s="16">
-        <v>1.3041666666666667</v>
+        <v>2.1736111111111112E-2</v>
       </c>
       <c r="F8" s="22">
-        <v>0.76666666666666661</v>
+        <v>1.2777777777777777E-2</v>
       </c>
       <c r="G8" s="21">
         <f t="shared" si="1"/>
-        <v>0.53750000000000009</v>
+        <v>8.9583333333333355E-3</v>
       </c>
       <c r="H8" s="16" t="s">
         <v>15</v>
@@ -1058,24 +1058,24 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C9" s="2">
-        <v>0.57500000000000007</v>
+        <v>9.5833333333333343E-3</v>
       </c>
       <c r="D9" s="15">
         <f t="shared" si="0"/>
-        <v>0.14097222222222217</v>
+        <v>2.3495370370370371E-3</v>
       </c>
       <c r="E9" s="16">
-        <v>0.71597222222222223</v>
+        <v>1.1932870370370371E-2</v>
       </c>
       <c r="F9" s="22">
-        <v>0.42430555555555555</v>
+        <v>7.0717592592592594E-3</v>
       </c>
       <c r="G9" s="22">
         <f t="shared" si="1"/>
-        <v>0.29166666666666669</v>
+        <v>4.8611111111111121E-3</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>13</v>
@@ -1085,53 +1085,61 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8.8657407407407417E-3</v>
+      </c>
+      <c r="D10" s="15">
+        <f t="shared" si="0"/>
+        <v>1.2847222222222218E-3</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1.0150462962962964E-2</v>
+      </c>
+      <c r="F10" s="22">
+        <v>4.2592592592592595E-3</v>
+      </c>
+      <c r="G10" s="22">
+        <f t="shared" si="1"/>
+        <v>5.8912037037037041E-3</v>
+      </c>
+      <c r="H10" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.53194444444444444</v>
-      </c>
-      <c r="D10" s="15">
-        <f t="shared" si="0"/>
-        <v>7.7083333333333393E-2</v>
-      </c>
-      <c r="E10" s="16">
-        <v>0.60902777777777783</v>
-      </c>
-      <c r="F10" s="22">
-        <v>0.25555555555555559</v>
-      </c>
-      <c r="G10" s="22">
-        <f t="shared" si="1"/>
-        <v>0.35347222222222224</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>98</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="2"/>
+        <v>98</v>
+      </c>
+      <c r="C11" s="2">
+        <v>9.8726851851851857E-3</v>
+      </c>
       <c r="D11" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="22"/>
+        <v>1.0810185185185187E-2</v>
+      </c>
+      <c r="E11" s="16">
+        <v>2.0682870370370372E-2</v>
+      </c>
+      <c r="F11" s="22">
+        <v>1.2199074074074072E-2</v>
+      </c>
       <c r="G11" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="16"/>
+        <v>8.4837962962963E-3</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="15">
@@ -1150,7 +1158,7 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="15">
@@ -1169,7 +1177,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1188,7 +1196,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1207,7 +1215,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1226,7 +1234,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1245,7 +1253,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1264,7 +1272,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1283,7 +1291,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1302,7 +1310,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1321,7 +1329,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1340,7 +1348,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1359,7 +1367,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1378,7 +1386,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1397,7 +1405,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1416,7 +1424,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1435,7 +1443,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1454,7 +1462,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Added Day 9 results to viz.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 9: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 10: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>9th</t>
+  </si>
+  <si>
+    <t>Day 9: Encoding Error</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,33 +1162,41 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C13" s="2">
+        <v>5.3240740740740748E-3</v>
+      </c>
       <c r="D13" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="22"/>
+        <v>6.2962962962962964E-3</v>
+      </c>
+      <c r="E13" s="16">
+        <v>1.1620370370370371E-2</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0.48541666666666666</v>
+      </c>
       <c r="G13" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="16"/>
+        <v>-0.47379629629629627</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="15">
@@ -1207,7 +1215,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1226,7 +1234,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1245,7 +1253,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1264,7 +1272,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1283,7 +1291,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1302,7 +1310,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1321,7 +1329,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1340,7 +1348,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1359,7 +1367,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1378,7 +1386,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1397,7 +1405,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1416,7 +1424,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1435,7 +1443,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1454,7 +1462,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1473,7 +1481,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Top 10 for Day 10.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 10: </t>
-  </si>
-  <si>
     <t>Day 11:</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 9: Encoding Error</t>
+  </si>
+  <si>
+    <t>Day 10: Adapter Array</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,26 +1196,34 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5.3240740740740748E-3</v>
+      </c>
       <c r="D14" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="16"/>
-      <c r="F14" s="22"/>
+        <v>1.5844907407407408E-2</v>
+      </c>
+      <c r="E14" s="16">
+        <v>2.1168981481481483E-2</v>
+      </c>
+      <c r="F14" s="22">
+        <v>1.6041666666666666E-2</v>
+      </c>
       <c r="G14" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="16"/>
+        <v>5.1273148148148172E-3</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="15">
@@ -1234,7 +1242,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1253,7 +1261,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1272,7 +1280,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1291,7 +1299,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1310,7 +1318,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1329,7 +1337,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1348,7 +1356,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1367,7 +1375,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1386,7 +1394,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1405,7 +1413,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1424,7 +1432,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1443,7 +1451,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1462,7 +1470,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1481,7 +1489,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Viz data for Day 11 so far.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t>Day 11:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 12: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 10: Adapter Array</t>
+  </si>
+  <si>
+    <t>Day 11: Seating System</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,26 +1223,34 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C15" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.503472222222222E-2</v>
+      </c>
       <c r="D15" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="16"/>
-      <c r="F15" s="22"/>
+        <v>9.3518518518518542E-3</v>
+      </c>
+      <c r="E15" s="16">
+        <v>2.4386574074074074E-2</v>
+      </c>
+      <c r="F15" s="22">
+        <v>1.5219907407407409E-2</v>
+      </c>
       <c r="G15" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="16"/>
+        <v>9.166666666666665E-3</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="15">
@@ -1261,7 +1269,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="15">
@@ -1280,7 +1288,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1299,7 +1307,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1318,7 +1326,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1337,7 +1345,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1356,7 +1364,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1375,7 +1383,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1394,7 +1402,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1413,7 +1421,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1432,7 +1440,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1451,7 +1459,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1470,7 +1478,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1489,7 +1497,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Viz update for Day 13.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 13: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 14: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 12: Rain Risk</t>
+  </si>
+  <si>
+    <t>Day 13: Shuttle Search</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,7 +1223,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" s="2">
         <v>1.503472222222222E-2</v>
@@ -1250,7 +1250,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C16" s="2">
         <v>1.357638888888889E-2</v>
@@ -1277,26 +1277,34 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C17" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C17" s="2">
+        <v>7.083333333333333E-3</v>
+      </c>
       <c r="D17" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="22"/>
+        <v>2.8368055555555553E-2</v>
+      </c>
+      <c r="E17" s="16">
+        <v>3.5451388888888886E-2</v>
+      </c>
+      <c r="F17" s="22">
+        <v>2.3668981481481485E-2</v>
+      </c>
       <c r="G17" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="16"/>
+        <v>1.1782407407407401E-2</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="15">
@@ -1315,7 +1323,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1334,7 +1342,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1353,7 +1361,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1372,7 +1380,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1391,7 +1399,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1410,7 +1418,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1429,7 +1437,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1448,7 +1456,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1467,7 +1475,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1486,7 +1494,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1505,7 +1513,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Stats for day 14.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 14: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 15: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 13: Shuttle Search</t>
+  </si>
+  <si>
+    <t>Day 14: Docking Data</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,7 +1223,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="2">
         <v>1.503472222222222E-2</v>
@@ -1250,7 +1250,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="2">
         <v>1.357638888888889E-2</v>
@@ -1277,7 +1277,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" s="2">
         <v>7.083333333333333E-3</v>
@@ -1304,26 +1304,34 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.2418981481481482E-2</v>
+      </c>
       <c r="D18" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="16"/>
-      <c r="F18" s="22"/>
+        <v>1.0636574074074073E-2</v>
+      </c>
+      <c r="E18" s="16">
+        <v>2.3055555555555555E-2</v>
+      </c>
+      <c r="F18" s="22">
+        <v>2.013888888888889E-2</v>
+      </c>
       <c r="G18" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H18" s="16"/>
+        <v>2.9166666666666646E-3</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="15">
@@ -1342,7 +1350,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1361,7 +1369,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1380,7 +1388,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1399,7 +1407,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1418,7 +1426,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1437,7 +1445,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1456,7 +1464,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1475,7 +1483,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1494,7 +1502,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1513,7 +1521,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Viz data for Day 15.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 15: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 16: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 14: Docking Data</t>
+  </si>
+  <si>
+    <t>Day 15: Rambunctious Recitation</t>
   </si>
 </sst>
 </file>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,7 +1223,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" s="2">
         <v>1.503472222222222E-2</v>
@@ -1250,7 +1250,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2">
         <v>1.357638888888889E-2</v>
@@ -1277,7 +1277,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C17" s="2">
         <v>7.083333333333333E-3</v>
@@ -1304,7 +1304,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C18" s="2">
         <v>1.2418981481481482E-2</v>
@@ -1331,26 +1331,34 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.1354166666666667E-2</v>
+      </c>
       <c r="D19" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="22"/>
+        <v>3.2638888888888891E-3</v>
+      </c>
+      <c r="E19" s="16">
+        <v>1.4618055555555556E-2</v>
+      </c>
+      <c r="F19" s="22">
+        <v>9.5023148148148159E-3</v>
+      </c>
       <c r="G19" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H19" s="16"/>
+        <v>5.1157407407407401E-3</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>9</v>
+      </c>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="15">
@@ -1369,7 +1377,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1388,7 +1396,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1407,7 +1415,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1426,7 +1434,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1445,7 +1453,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1464,7 +1472,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1483,7 +1491,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1502,7 +1510,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1521,7 +1529,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Updated viz with Day 16 results.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 16: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 17: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 15: Rambunctious Recitation</t>
+  </si>
+  <si>
+    <t>Day 16: Ticket Translation</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,7 +1223,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="2">
         <v>1.503472222222222E-2</v>
@@ -1250,7 +1250,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" s="2">
         <v>1.357638888888889E-2</v>
@@ -1277,7 +1277,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2">
         <v>7.083333333333333E-3</v>
@@ -1304,7 +1304,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C18" s="2">
         <v>1.2418981481481482E-2</v>
@@ -1331,7 +1331,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="2">
         <v>1.1354166666666667E-2</v>
@@ -1358,26 +1358,34 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1.7951388888888888E-2</v>
+      </c>
       <c r="D20" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="22"/>
+        <v>1.3599537037037032E-2</v>
+      </c>
+      <c r="E20" s="16">
+        <v>3.155092592592592E-2</v>
+      </c>
+      <c r="F20" s="22">
+        <v>2.0370370370370369E-2</v>
+      </c>
       <c r="G20" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H20" s="16"/>
+        <v>1.1180555555555551E-2</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="15">
@@ -1396,7 +1404,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1415,7 +1423,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1434,7 +1442,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1453,7 +1461,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1472,7 +1480,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1491,7 +1499,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1510,7 +1518,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1529,7 +1537,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Viz data for day 17.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 17: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 18: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 16: Ticket Translation</t>
+  </si>
+  <si>
+    <t>Day 17: Conway Cubes</t>
   </si>
 </sst>
 </file>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,7 +1223,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2">
         <v>1.503472222222222E-2</v>
@@ -1250,7 +1250,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="2">
         <v>1.357638888888889E-2</v>
@@ -1277,7 +1277,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2">
         <v>7.083333333333333E-3</v>
@@ -1304,7 +1304,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2">
         <v>1.2418981481481482E-2</v>
@@ -1331,7 +1331,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" s="2">
         <v>1.1354166666666667E-2</v>
@@ -1358,7 +1358,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" s="2">
         <v>1.7951388888888888E-2</v>
@@ -1385,26 +1385,34 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4.0682870370370376E-2</v>
+      </c>
       <c r="D21" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="16"/>
-      <c r="F21" s="22"/>
+        <v>3.0787037037037016E-3</v>
+      </c>
+      <c r="E21" s="16">
+        <v>4.3761574074074078E-2</v>
+      </c>
+      <c r="F21" s="22">
+        <v>1.269675925925926E-2</v>
+      </c>
       <c r="G21" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H21" s="16"/>
+        <v>3.1064814814814816E-2</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="15">
@@ -1423,7 +1431,7 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1442,7 +1450,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1461,7 +1469,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1480,7 +1488,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1499,7 +1507,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1518,7 +1526,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1537,7 +1545,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
added console message showing most recent time on most recent day (avoid unnecessary PUTs to S3).
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 18: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 19: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 17: Conway Cubes</t>
+  </si>
+  <si>
+    <t>Day 18: Operation Order</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,7 +1223,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="2">
         <v>1.503472222222222E-2</v>
@@ -1250,7 +1250,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="2">
         <v>1.357638888888889E-2</v>
@@ -1277,7 +1277,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="2">
         <v>7.083333333333333E-3</v>
@@ -1304,7 +1304,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="2">
         <v>1.2418981481481482E-2</v>
@@ -1331,7 +1331,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="2">
         <v>1.1354166666666667E-2</v>
@@ -1358,7 +1358,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C20" s="2">
         <v>1.7951388888888888E-2</v>
@@ -1385,7 +1385,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="2">
         <v>4.0682870370370376E-2</v>
@@ -1412,26 +1412,34 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C22" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C22" s="2">
+        <v>9.7337962962962977E-3</v>
+      </c>
       <c r="D22" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="22"/>
+        <v>9.6296296296296286E-3</v>
+      </c>
+      <c r="E22" s="16">
+        <v>1.9363425925925926E-2</v>
+      </c>
+      <c r="F22" s="22">
+        <v>1.4247685185185184E-2</v>
+      </c>
       <c r="G22" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H22" s="16"/>
+        <v>5.1157407407407419E-3</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="15">
@@ -1450,7 +1458,7 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1469,7 +1477,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1488,7 +1496,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1507,7 +1515,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1526,7 +1534,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1545,7 +1553,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>

<commit_message>
Viz data for day 19.
</commit_message>
<xml_diff>
--- a/data/viz/personalStats.xlsx
+++ b/data/viz/personalStats.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="100">
   <si>
     <t>Puzzle</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Day 25: Cryostasis</t>
   </si>
   <si>
-    <t xml:space="preserve">Day 19: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Day 20: </t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>Day 18: Operation Order</t>
+  </si>
+  <si>
+    <t>Day 19: Monster Messages</t>
   </si>
 </sst>
 </file>
@@ -871,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +953,7 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="2">
         <v>4.8495370370370368E-3</v>
@@ -980,7 +980,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="2">
         <v>2.9861111111111113E-3</v>
@@ -1007,7 +1007,7 @@
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2">
         <v>6.3888888888888884E-3</v>
@@ -1034,7 +1034,7 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="2">
         <v>9.1435185185185178E-3</v>
@@ -1061,7 +1061,7 @@
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="2">
         <v>9.5833333333333343E-3</v>
@@ -1088,7 +1088,7 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="2">
         <v>8.8657407407407417E-3</v>
@@ -1108,14 +1108,14 @@
         <v>5.8912037037037041E-3</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I10" s="4"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" s="2">
         <v>9.8726851851851857E-3</v>
@@ -1142,7 +1142,7 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" s="2">
         <v>5.3819444444444453E-3</v>
@@ -1162,14 +1162,14 @@
         <v>7.4652777777777773E-3</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I12" s="4"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1196,7 +1196,7 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C14" s="2">
         <v>5.3240740740740748E-3</v>
@@ -1223,7 +1223,7 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" s="2">
         <v>1.503472222222222E-2</v>
@@ -1250,7 +1250,7 @@
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" s="2">
         <v>1.357638888888889E-2</v>
@@ -1277,7 +1277,7 @@
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2">
         <v>7.083333333333333E-3</v>
@@ -1304,7 +1304,7 @@
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2">
         <v>1.2418981481481482E-2</v>
@@ -1331,7 +1331,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2">
         <v>1.1354166666666667E-2</v>
@@ -1358,7 +1358,7 @@
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" s="2">
         <v>1.7951388888888888E-2</v>
@@ -1385,7 +1385,7 @@
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" s="2">
         <v>4.0682870370370376E-2</v>
@@ -1412,7 +1412,7 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2">
         <v>9.7337962962962977E-3</v>
@@ -1439,26 +1439,34 @@
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C23" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2.1886574074074072E-2</v>
+      </c>
       <c r="D23" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="22"/>
+        <v>3.1817129629629626E-2</v>
+      </c>
+      <c r="E23" s="16">
+        <v>5.3703703703703698E-2</v>
+      </c>
+      <c r="F23" s="22">
+        <v>3.9039351851851853E-2</v>
+      </c>
       <c r="G23" s="22">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="16"/>
+        <v>1.4664351851851845E-2</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="15">
@@ -1477,7 +1485,7 @@
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="15">
@@ -1496,7 +1504,7 @@
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="15">
@@ -1515,7 +1523,7 @@
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="15">
@@ -1534,7 +1542,7 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15">
@@ -1553,7 +1561,7 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="15">

</xml_diff>